<commit_message>
Added all results for Celtra cases without change point detection in: Results.xlsx
</commit_message>
<xml_diff>
--- a/matlab_analysis/Results.xlsx
+++ b/matlab_analysis/Results.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="49">
   <si>
     <t>conf</t>
   </si>
@@ -67,9 +67,6 @@
     <t xml:space="preserve">experiment_filenames{12}   = 'Jackpot_init.pyc_2014_10_18_01_24_57';    %complete with own testcase11, was run by mistake   </t>
   </si>
   <si>
-    <t>experiment_filenames{13}   = '';</t>
-  </si>
-  <si>
     <t>experiment_filenames{14}   = '';</t>
   </si>
   <si>
@@ -97,63 +94,24 @@
     <t>%no change point experiments: all strategies on Celtra cases (T1 cases 0-4, T2 cases 5-9, T2 cases 0-9), Or - oracle 0/1</t>
   </si>
   <si>
-    <t>experiment_filenames{15}   = '';</t>
-  </si>
-  <si>
-    <t>experiment_filenames{16}   = '';</t>
-  </si>
-  <si>
-    <t>experiment_filenames{17}   = '';</t>
-  </si>
-  <si>
     <t>experiment_filenames{18}   = '';</t>
   </si>
   <si>
-    <t>experiment_filenames{19}   = '';</t>
-  </si>
-  <si>
-    <t>experiment_filenames{20}   = '';</t>
-  </si>
-  <si>
-    <t>experiment_filenames{21}   = '';</t>
-  </si>
-  <si>
     <t>experiment_filenames{22}   = '';</t>
   </si>
   <si>
-    <t>experiment_filenames{23}   = '';</t>
-  </si>
-  <si>
-    <t>experiment_filenames{24}   = '';</t>
-  </si>
-  <si>
-    <t>experiment_filenames{25}   = '';</t>
-  </si>
-  <si>
     <t>experiment_filenames{26}   = '';</t>
   </si>
   <si>
-    <t>experiment_filenames{27}   = '';</t>
-  </si>
-  <si>
-    <t>experiment_filenames{28}   = '';</t>
-  </si>
-  <si>
     <t>experiment_filenames{29}   = 'Reprint___2014_10_18_EG_T3_Or0___2014_10_18_23_57_07';</t>
   </si>
   <si>
-    <t>experiment_filenames{30}   = 'Reprint___2014_10_18_EG_T3_Or1___2014_10_18_23_57_10';</t>
-  </si>
-  <si>
     <t>experiment_filenames{31}   = 'Reprint___2014_10_18_UCB1_T3_Or0___2014_10_18_12_35_45';</t>
   </si>
   <si>
     <t>experiment_filenames{32}   = 'Reprint___2014_10_18_UCBT_T3_Or0___2014_10_18_12_36_16';</t>
   </si>
   <si>
-    <t>experiment_filenames{33}   = 'Reprint___2014_10_18_SMAX_T3_Or0___2014_10_18_23_57_12';</t>
-  </si>
-  <si>
     <t>experiment_filenames{34}   = 'Reprint___2014_10_18_SMAX_T3_Or1___2014_10_18_21_38_03';</t>
   </si>
   <si>
@@ -163,7 +121,46 @@
     <t>experiment_filenames{36}   = 'Reprint___2014_10_18_UCBT_T3_Or1___2014_10_18_12_37_21';</t>
   </si>
   <si>
-    <t>0.210 - 0.240</t>
+    <t>experiment_filenames{13}   = 'Reprint___2014_10_18_EG_T1_Or0___2014_10_19_01_50_01';</t>
+  </si>
+  <si>
+    <t>experiment_filenames{17}   = 'Reprint___2014_10_18_EG_T1_Or1___2014_10_19_01_50_04';</t>
+  </si>
+  <si>
+    <t>experiment_filenames{21}   = 'Reprint___2014_10_18_EG_T2_Or0___2014_10_19_01_50_06';</t>
+  </si>
+  <si>
+    <t>experiment_filenames{25}   = 'Reprint___2014_10_18_EG_T2_Or1___2014_10_19_01_50_08';</t>
+  </si>
+  <si>
+    <t>experiment_filenames{30}   = 'Reprint___2014_10_18_SMAX_T3_Or0___2014_10_19_00_42_42';</t>
+  </si>
+  <si>
+    <t>experiment_filenames{33}   = 'Reprint___2014_10_18_EG_T3_Or1___2014_10_18_23_57_10';</t>
+  </si>
+  <si>
+    <t>experiment_filenames{15}   = 'Reprint___2014_10_18_UCB1_T1_Or0___2014_10_19_01_50_10';</t>
+  </si>
+  <si>
+    <t>experiment_filenames{16}   = 'Reprint___2014_10_18_UCBT_T1_Or0___2014_10_19_01_50_34';</t>
+  </si>
+  <si>
+    <t>experiment_filenames{19}   = 'Reprint___2014_10_18_UCB1_T1_Or1___2014_10_19_01_50_11';</t>
+  </si>
+  <si>
+    <t>experiment_filenames{20}   = 'Reprint___2014_10_18_UCBT_T1_Or1___2014_10_19_01_50_38';</t>
+  </si>
+  <si>
+    <t>experiment_filenames{23}   = 'Reprint___2014_10_18_UCB1_T2_Or0___2014_10_19_01_50_13';</t>
+  </si>
+  <si>
+    <t>experiment_filenames{24}   = 'Reprint___2014_10_18_UCBT_T2_Or0___2014_10_19_01_50_41';</t>
+  </si>
+  <si>
+    <t>experiment_filenames{27}   = 'Reprint___2014_10_18_UCB1_T2_Or1___2014_10_19_01_50_15';</t>
+  </si>
+  <si>
+    <t>experiment_filenames{28}   = 'Reprint___2014_10_18_UCBT_T2_Or1___2014_10_19_01_50_44';</t>
   </si>
 </sst>
 </file>
@@ -612,8 +609,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M422"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B21" workbookViewId="0">
-      <selection activeCell="G46" sqref="G46"/>
+    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
+      <selection activeCell="M52" sqref="M52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -660,7 +657,7 @@
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="M5" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
@@ -680,19 +677,19 @@
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" s="15" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B10" s="15" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C10" s="15" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D10" s="15" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E10" s="15" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="M10" s="1" t="s">
         <v>8</v>
@@ -705,7 +702,7 @@
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="M13" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.25">
@@ -757,109 +754,193 @@
     </row>
     <row r="22" spans="5:13" x14ac:dyDescent="0.25">
       <c r="M22" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="23" spans="5:13" x14ac:dyDescent="0.25">
+      <c r="E23" s="13">
+        <v>0.12</v>
+      </c>
+      <c r="G23" s="11">
+        <v>73.400000000000006</v>
+      </c>
       <c r="M23" s="1" t="s">
-        <v>17</v>
+        <v>35</v>
       </c>
     </row>
     <row r="24" spans="5:13" x14ac:dyDescent="0.25">
       <c r="M24" s="7" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="25" spans="5:13" x14ac:dyDescent="0.25">
+      <c r="E25" s="13">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="G25" s="11">
+        <v>68.900000000000006</v>
+      </c>
       <c r="M25" s="1" t="s">
-        <v>27</v>
+        <v>41</v>
       </c>
     </row>
     <row r="26" spans="5:13" x14ac:dyDescent="0.25">
+      <c r="E26" s="13">
+        <v>0.35</v>
+      </c>
+      <c r="G26" s="11">
+        <v>71.7</v>
+      </c>
       <c r="M26" s="1" t="s">
-        <v>28</v>
+        <v>42</v>
       </c>
     </row>
     <row r="27" spans="5:13" x14ac:dyDescent="0.25">
+      <c r="E27" s="13">
+        <v>3.5999999999999997E-2</v>
+      </c>
+      <c r="G27" s="11">
+        <v>94.1</v>
+      </c>
       <c r="M27" s="1" t="s">
-        <v>29</v>
+        <v>36</v>
       </c>
     </row>
     <row r="28" spans="5:13" x14ac:dyDescent="0.25">
       <c r="M28" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
     </row>
     <row r="29" spans="5:13" x14ac:dyDescent="0.25">
+      <c r="E29" s="13">
+        <v>0</v>
+      </c>
+      <c r="G29" s="11">
+        <v>99.83</v>
+      </c>
       <c r="M29" s="1" t="s">
-        <v>31</v>
+        <v>43</v>
       </c>
     </row>
     <row r="30" spans="5:13" x14ac:dyDescent="0.25">
+      <c r="E30" s="13">
+        <v>0</v>
+      </c>
+      <c r="G30" s="11">
+        <v>99.83</v>
+      </c>
       <c r="M30" s="1" t="s">
-        <v>32</v>
+        <v>44</v>
       </c>
     </row>
     <row r="31" spans="5:13" x14ac:dyDescent="0.25">
       <c r="M31" s="2"/>
     </row>
     <row r="32" spans="5:13" x14ac:dyDescent="0.25">
+      <c r="E32" s="13">
+        <v>0.06</v>
+      </c>
+      <c r="G32" s="11">
+        <v>35.6</v>
+      </c>
       <c r="M32" s="7" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
     </row>
     <row r="33" spans="5:13" x14ac:dyDescent="0.25">
       <c r="M33" s="7" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
     </row>
     <row r="34" spans="5:13" x14ac:dyDescent="0.25">
+      <c r="E34" s="13">
+        <v>0.34</v>
+      </c>
+      <c r="G34" s="11">
+        <v>62.5</v>
+      </c>
       <c r="M34" s="7" t="s">
-        <v>35</v>
+        <v>45</v>
       </c>
     </row>
     <row r="35" spans="5:13" x14ac:dyDescent="0.25">
+      <c r="E35" s="13">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="G35" s="11">
+        <v>64.099999999999994</v>
+      </c>
       <c r="M35" s="7" t="s">
-        <v>36</v>
+        <v>46</v>
       </c>
     </row>
     <row r="36" spans="5:13" x14ac:dyDescent="0.25">
+      <c r="E36" s="13">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="G36" s="11">
+        <v>43.8</v>
+      </c>
       <c r="M36" s="7" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="37" spans="5:13" x14ac:dyDescent="0.25">
       <c r="M37" s="7" t="s">
-        <v>38</v>
+        <v>28</v>
       </c>
     </row>
     <row r="38" spans="5:13" x14ac:dyDescent="0.25">
+      <c r="E38" s="13">
+        <v>8.5000000000000006E-2</v>
+      </c>
+      <c r="G38" s="11">
+        <v>83.6</v>
+      </c>
       <c r="M38" s="7" t="s">
-        <v>39</v>
+        <v>47</v>
       </c>
     </row>
     <row r="39" spans="5:13" x14ac:dyDescent="0.25">
+      <c r="E39" s="13">
+        <v>0.23</v>
+      </c>
+      <c r="G39" s="11">
+        <v>82.25</v>
+      </c>
       <c r="M39" s="7" t="s">
-        <v>40</v>
+        <v>48</v>
       </c>
     </row>
     <row r="40" spans="5:13" x14ac:dyDescent="0.25">
       <c r="M40" s="7"/>
     </row>
     <row r="41" spans="5:13" x14ac:dyDescent="0.25">
+      <c r="E41" s="13">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="G41" s="11">
+        <v>48.3</v>
+      </c>
       <c r="M41" s="7" t="s">
-        <v>41</v>
+        <v>29</v>
       </c>
     </row>
     <row r="42" spans="5:13" x14ac:dyDescent="0.25">
+      <c r="E42" s="13">
+        <v>1E-3</v>
+      </c>
+      <c r="G42" s="11">
+        <v>30.7</v>
+      </c>
       <c r="J42" s="4"/>
       <c r="M42" s="7" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
     </row>
     <row r="43" spans="5:13" x14ac:dyDescent="0.25">
-      <c r="E43" s="13" t="s">
-        <v>49</v>
+      <c r="E43" s="13">
+        <v>0.24</v>
       </c>
       <c r="F43" s="10"/>
       <c r="G43" s="11">
@@ -867,7 +948,7 @@
       </c>
       <c r="H43" s="4"/>
       <c r="M43" s="7" t="s">
-        <v>43</v>
+        <v>30</v>
       </c>
     </row>
     <row r="44" spans="5:13" x14ac:dyDescent="0.25">
@@ -878,17 +959,29 @@
         <v>61.07</v>
       </c>
       <c r="M44" s="7" t="s">
-        <v>44</v>
+        <v>31</v>
       </c>
     </row>
     <row r="45" spans="5:13" x14ac:dyDescent="0.25">
+      <c r="E45" s="13">
+        <v>0.02</v>
+      </c>
+      <c r="G45" s="11">
+        <v>64.3</v>
+      </c>
       <c r="M45" s="7" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
     </row>
     <row r="46" spans="5:13" x14ac:dyDescent="0.25">
+      <c r="E46" s="13">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="G46" s="11">
+        <v>34.4</v>
+      </c>
       <c r="M46" s="7" t="s">
-        <v>46</v>
+        <v>32</v>
       </c>
     </row>
     <row r="47" spans="5:13" x14ac:dyDescent="0.25">
@@ -899,7 +992,7 @@
         <v>76.790000000000006</v>
       </c>
       <c r="M47" s="7" t="s">
-        <v>47</v>
+        <v>33</v>
       </c>
     </row>
     <row r="48" spans="5:13" x14ac:dyDescent="0.25">
@@ -910,7 +1003,7 @@
         <v>76.64</v>
       </c>
       <c r="M48" s="7" t="s">
-        <v>48</v>
+        <v>34</v>
       </c>
     </row>
     <row r="49" spans="4:13" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Improvement to Optimization.py output Added first results for DavorTom changePointDetection
</commit_message>
<xml_diff>
--- a/matlab_analysis/Results.xlsx
+++ b/matlab_analysis/Results.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="63">
   <si>
     <t>conf</t>
   </si>
@@ -161,6 +161,48 @@
   </si>
   <si>
     <t>experiment_filenames{28}   = 'Reprint___2014_10_18_UCBT_T2_Or1___2014_10_19_01_50_44';</t>
+  </si>
+  <si>
+    <t>%DavorTom change point experiments</t>
+  </si>
+  <si>
+    <t>experiment_filenames{37}   = 'Reprint___2014_10_20_UCBT_T3_Or1_parTHR_ResetZero___2014_10_20_01_24_54';</t>
+  </si>
+  <si>
+    <t>experiment_filenames{38}   = 'Reprint___2014_10_20_UCBT_T3_Or1_parTHR_ResetAllMA___2014_10_20_01_24_47';</t>
+  </si>
+  <si>
+    <t>experiment_filenames{39}   = 'Reprint___2014_10_20_UCBT_T3_Or1_parTHR_ResetCut___2014_10_20_01_24_49';</t>
+  </si>
+  <si>
+    <t>experiment_filenames{40}   = 'Reprint___2014_10_20_UCBT_T3_Or1_parTHR_ResetSingle___2014_10_20_01_24_52';</t>
+  </si>
+  <si>
+    <t>experiment_filenames{41}   = 'Reprint___2014_10_20_UCBT_T3_Or0_Shr1.0_Min50_ResetZero___2014_10_20_00_01_05';</t>
+  </si>
+  <si>
+    <t>experiment_filenames{42}   = 'Reprint___2014_10_20_UCBT_T3_Or0_Shr1.0_Min50_ResetAllMA___2014_10_20_00_01_50';</t>
+  </si>
+  <si>
+    <t>experiment_filenames{43}   = 'Reprint___2014_10_20_UCBT_T3_Or0_Shr1.0_Min50_ResetCut___2014_10_20_00_02_16';</t>
+  </si>
+  <si>
+    <t>experiment_filenames{44}   = 'Reprint___2014_10_20_UCBT_T3_Or0_Shr1.0_Min50_ResetSingle___2014_10_20_00_02_45';</t>
+  </si>
+  <si>
+    <t>experiment_filenames{45}   = 'Reprint___2014_10_20_UCBT_T3_Or0_4par_ResetZero___2014_10_20_01_25_55';</t>
+  </si>
+  <si>
+    <t>experiment_filenames{46}   = 'Reprint___2014_10_20_UCBT_T3_Or0_4par_ResetAllMA___2014_10_20_01_25_30';</t>
+  </si>
+  <si>
+    <t>experiment_filenames{47}   = 'Reprint___2014_10_20_UCBT_T3_Or0_4par_ResetCut___2014_10_20_01_25_39';</t>
+  </si>
+  <si>
+    <t>experiment_filenames{48}   = 'Reprint___2014_10_20_UCBT_T3_Or0_4par_ResetSingle___2014_10_20_01_25_51';</t>
+  </si>
+  <si>
+    <t>max 7</t>
   </si>
 </sst>
 </file>
@@ -171,7 +213,7 @@
     <numFmt numFmtId="164" formatCode="0.0"/>
     <numFmt numFmtId="165" formatCode="0.000"/>
   </numFmts>
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -243,6 +285,30 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="4"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="9"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="238"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="9"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="238"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -264,7 +330,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -301,6 +367,13 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="165" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
   </cellXfs>
@@ -609,8 +682,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M422"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
-      <selection activeCell="M52" sqref="M52"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="I25" sqref="I25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -618,7 +691,7 @@
     <col min="1" max="5" width="8" style="13" customWidth="1"/>
     <col min="6" max="6" width="8" customWidth="1"/>
     <col min="7" max="7" width="11.7109375" style="11" customWidth="1"/>
-    <col min="8" max="8" width="5.5703125" style="5" customWidth="1"/>
+    <col min="8" max="8" width="5.5703125" style="21" customWidth="1"/>
     <col min="9" max="9" width="2.7109375" style="5" customWidth="1"/>
     <col min="10" max="11" width="5.5703125" style="5" customWidth="1"/>
     <col min="12" max="12" width="1.5703125" style="5" customWidth="1"/>
@@ -640,7 +713,7 @@
       <c r="G2" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="H2" s="4" t="s">
+      <c r="H2" s="22" t="s">
         <v>0</v>
       </c>
       <c r="I2" s="4"/>
@@ -946,7 +1019,9 @@
       <c r="G43" s="11">
         <v>58.7</v>
       </c>
-      <c r="H43" s="4"/>
+      <c r="H43" s="21">
+        <v>0.7</v>
+      </c>
       <c r="M43" s="7" t="s">
         <v>30</v>
       </c>
@@ -958,6 +1033,9 @@
       <c r="G44" s="11">
         <v>61.07</v>
       </c>
+      <c r="H44" s="21">
+        <v>0.6</v>
+      </c>
       <c r="M44" s="7" t="s">
         <v>31</v>
       </c>
@@ -991,6 +1069,9 @@
       <c r="G47" s="11">
         <v>76.790000000000006</v>
       </c>
+      <c r="H47" s="21">
+        <v>0.2</v>
+      </c>
       <c r="M47" s="7" t="s">
         <v>33</v>
       </c>
@@ -1002,6 +1083,9 @@
       <c r="G48" s="11">
         <v>76.64</v>
       </c>
+      <c r="H48" s="21">
+        <v>0.1</v>
+      </c>
       <c r="M48" s="7" t="s">
         <v>34</v>
       </c>
@@ -1010,48 +1094,183 @@
       <c r="M49" s="7"/>
     </row>
     <row r="50" spans="4:13" x14ac:dyDescent="0.25">
-      <c r="M50" s="7"/>
+      <c r="M50" s="2" t="s">
+        <v>49</v>
+      </c>
     </row>
     <row r="51" spans="4:13" x14ac:dyDescent="0.25">
-      <c r="M51" s="7"/>
+      <c r="E51" s="13">
+        <v>3.82</v>
+      </c>
+      <c r="G51" s="11">
+        <v>60.2</v>
+      </c>
+      <c r="M51" s="7" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="52" spans="4:13" x14ac:dyDescent="0.25">
-      <c r="M52" s="7"/>
+      <c r="E52" s="13">
+        <v>3.34</v>
+      </c>
+      <c r="G52" s="11">
+        <v>60.9</v>
+      </c>
+      <c r="M52" s="7" t="s">
+        <v>51</v>
+      </c>
     </row>
     <row r="53" spans="4:13" x14ac:dyDescent="0.25">
-      <c r="M53" s="7"/>
+      <c r="E53" s="13">
+        <v>3.33</v>
+      </c>
+      <c r="G53" s="11">
+        <v>60.1</v>
+      </c>
+      <c r="M53" s="7" t="s">
+        <v>52</v>
+      </c>
     </row>
     <row r="54" spans="4:13" x14ac:dyDescent="0.25">
-      <c r="M54" s="7"/>
+      <c r="E54" s="13">
+        <v>0.51</v>
+      </c>
+      <c r="G54" s="11">
+        <v>66.7</v>
+      </c>
+      <c r="M54" s="7" t="s">
+        <v>53</v>
+      </c>
     </row>
     <row r="55" spans="4:13" x14ac:dyDescent="0.25">
+      <c r="D55" s="20" t="s">
+        <v>62</v>
+      </c>
       <c r="J55" s="4"/>
       <c r="M55" s="7"/>
     </row>
     <row r="56" spans="4:13" x14ac:dyDescent="0.25">
+      <c r="D56" s="13">
+        <v>6</v>
+      </c>
+      <c r="E56" s="13">
+        <v>0.55000000000000004</v>
+      </c>
       <c r="F56" s="10"/>
-      <c r="G56" s="12"/>
-      <c r="H56" s="4"/>
+      <c r="G56" s="11">
+        <v>54.2</v>
+      </c>
+      <c r="H56" s="21">
+        <v>0.1</v>
+      </c>
       <c r="I56" s="4"/>
       <c r="J56" s="4"/>
-      <c r="M56" s="7"/>
+      <c r="M56" s="7" t="s">
+        <v>54</v>
+      </c>
     </row>
     <row r="57" spans="4:13" x14ac:dyDescent="0.25">
+      <c r="D57" s="13">
+        <v>6</v>
+      </c>
+      <c r="E57" s="13">
+        <v>0.75</v>
+      </c>
       <c r="F57" s="4"/>
+      <c r="G57" s="11">
+        <v>55.7</v>
+      </c>
+      <c r="H57" s="21">
+        <v>1</v>
+      </c>
       <c r="I57" s="4"/>
       <c r="J57" s="4"/>
-      <c r="M57" s="7"/>
+      <c r="M57" s="7" t="s">
+        <v>55</v>
+      </c>
     </row>
     <row r="58" spans="4:13" x14ac:dyDescent="0.25">
+      <c r="D58" s="13">
+        <v>6.2</v>
+      </c>
+      <c r="E58" s="13">
+        <v>0.52</v>
+      </c>
       <c r="F58" s="4"/>
-      <c r="M58" s="7"/>
+      <c r="G58" s="11">
+        <v>54.6</v>
+      </c>
+      <c r="H58" s="21">
+        <v>0.3</v>
+      </c>
+      <c r="M58" s="7" t="s">
+        <v>56</v>
+      </c>
     </row>
     <row r="59" spans="4:13" x14ac:dyDescent="0.25">
-      <c r="M59" s="7"/>
+      <c r="D59" s="13">
+        <v>4.45</v>
+      </c>
+      <c r="E59" s="13">
+        <v>0.79</v>
+      </c>
+      <c r="G59" s="11">
+        <v>59.6</v>
+      </c>
+      <c r="H59" s="21">
+        <v>0.6</v>
+      </c>
+      <c r="M59" s="7" t="s">
+        <v>57</v>
+      </c>
     </row>
     <row r="60" spans="4:13" x14ac:dyDescent="0.25">
       <c r="D60" s="16"/>
       <c r="M60" s="7"/>
+    </row>
+    <row r="61" spans="4:13" x14ac:dyDescent="0.25">
+      <c r="G61" s="11">
+        <v>56.1</v>
+      </c>
+      <c r="H61" s="21">
+        <v>0.5</v>
+      </c>
+      <c r="M61" s="1" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="62" spans="4:13" x14ac:dyDescent="0.25">
+      <c r="G62" s="11">
+        <v>56.2</v>
+      </c>
+      <c r="H62" s="21">
+        <v>2.6</v>
+      </c>
+      <c r="M62" s="1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="63" spans="4:13" x14ac:dyDescent="0.25">
+      <c r="G63" s="11">
+        <v>55.1</v>
+      </c>
+      <c r="H63" s="21">
+        <v>0.2</v>
+      </c>
+      <c r="M63" s="1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="64" spans="4:13" x14ac:dyDescent="0.25">
+      <c r="G64" s="11">
+        <v>55.6</v>
+      </c>
+      <c r="H64" s="21">
+        <v>0.2</v>
+      </c>
+      <c r="M64" s="1" t="s">
+        <v>61</v>
+      </c>
     </row>
     <row r="65" spans="6:13" x14ac:dyDescent="0.25">
       <c r="F65" s="4"/>

</xml_diff>

<commit_message>
Improved mainAnalyseData.m Added paper
</commit_message>
<xml_diff>
--- a/matlab_analysis/Results.xlsx
+++ b/matlab_analysis/Results.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="80">
   <si>
     <t>conf</t>
   </si>
@@ -233,6 +233,27 @@
   </si>
   <si>
     <t>UCB_C</t>
+  </si>
+  <si>
+    <t>case7</t>
+  </si>
+  <si>
+    <t>case8</t>
+  </si>
+  <si>
+    <t>case9</t>
+  </si>
+  <si>
+    <t>case10</t>
+  </si>
+  <si>
+    <t>avg</t>
+  </si>
+  <si>
+    <t>min 0.5</t>
+  </si>
+  <si>
+    <t>cases</t>
   </si>
 </sst>
 </file>
@@ -243,7 +264,7 @@
     <numFmt numFmtId="164" formatCode="0.0"/>
     <numFmt numFmtId="165" formatCode="0.000"/>
   </numFmts>
-  <fonts count="12" x14ac:knownFonts="1">
+  <fonts count="14" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -339,6 +360,24 @@
       <charset val="238"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="4"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="238"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="238"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -360,7 +399,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -405,6 +444,9 @@
     <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="165" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -709,10 +751,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M422"/>
+  <dimension ref="A1:AJ422"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B41" workbookViewId="0">
-      <selection activeCell="F69" sqref="F69"/>
+    <sheetView tabSelected="1" topLeftCell="X51" workbookViewId="0">
+      <selection activeCell="AI80" sqref="AI80"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1303,7 +1345,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="65" spans="4:13" x14ac:dyDescent="0.25">
+    <row r="65" spans="4:36" x14ac:dyDescent="0.25">
       <c r="D65" s="19" t="s">
         <v>70</v>
       </c>
@@ -1311,7 +1353,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="66" spans="4:13" x14ac:dyDescent="0.25">
+    <row r="66" spans="4:36" x14ac:dyDescent="0.25">
       <c r="D66" s="13">
         <v>1.8</v>
       </c>
@@ -1329,7 +1371,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="67" spans="4:13" x14ac:dyDescent="0.25">
+    <row r="67" spans="4:36" x14ac:dyDescent="0.25">
       <c r="D67" s="13">
         <v>2.2999999999999998</v>
       </c>
@@ -1347,7 +1389,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="68" spans="4:13" x14ac:dyDescent="0.25">
+    <row r="68" spans="4:36" x14ac:dyDescent="0.25">
       <c r="D68" s="13">
         <v>2.2000000000000002</v>
       </c>
@@ -1365,7 +1407,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="69" spans="4:13" x14ac:dyDescent="0.25">
+    <row r="69" spans="4:36" x14ac:dyDescent="0.25">
       <c r="D69" s="13">
         <v>0.5</v>
       </c>
@@ -1381,8 +1423,16 @@
       <c r="M69" s="7" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="70" spans="4:13" x14ac:dyDescent="0.25">
+      <c r="AC69" s="22" t="s">
+        <v>79</v>
+      </c>
+      <c r="AD69" s="22"/>
+      <c r="AE69" s="22"/>
+      <c r="AF69" s="22"/>
+      <c r="AG69" s="22"/>
+      <c r="AH69" s="22"/>
+    </row>
+    <row r="70" spans="4:36" x14ac:dyDescent="0.25">
       <c r="D70" s="19" t="s">
         <v>71</v>
       </c>
@@ -1390,8 +1440,41 @@
         <v>70</v>
       </c>
       <c r="M70" s="7"/>
-    </row>
-    <row r="71" spans="4:13" x14ac:dyDescent="0.25">
+      <c r="Y70" s="22" t="s">
+        <v>73</v>
+      </c>
+      <c r="Z70" s="22" t="s">
+        <v>74</v>
+      </c>
+      <c r="AA70" s="22" t="s">
+        <v>75</v>
+      </c>
+      <c r="AB70" s="22" t="s">
+        <v>76</v>
+      </c>
+      <c r="AC70" s="22">
+        <v>1</v>
+      </c>
+      <c r="AD70" s="22">
+        <v>2</v>
+      </c>
+      <c r="AE70" s="22">
+        <v>3</v>
+      </c>
+      <c r="AF70" s="22">
+        <v>4</v>
+      </c>
+      <c r="AG70" s="22">
+        <v>5</v>
+      </c>
+      <c r="AH70" s="22">
+        <v>6</v>
+      </c>
+      <c r="AJ70" s="22" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="71" spans="4:36" x14ac:dyDescent="0.25">
       <c r="D71" s="13">
         <v>0.65500000000000003</v>
       </c>
@@ -1407,8 +1490,39 @@
       <c r="M71" s="1" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="72" spans="4:13" x14ac:dyDescent="0.25">
+      <c r="Y71">
+        <v>93.3</v>
+      </c>
+      <c r="Z71">
+        <v>97.9</v>
+      </c>
+      <c r="AB71">
+        <v>82.1</v>
+      </c>
+      <c r="AC71">
+        <v>99.6</v>
+      </c>
+      <c r="AD71">
+        <v>95.08</v>
+      </c>
+      <c r="AE71">
+        <v>97.4</v>
+      </c>
+      <c r="AF71">
+        <v>63.76</v>
+      </c>
+      <c r="AG71">
+        <v>10.57</v>
+      </c>
+      <c r="AH71">
+        <v>99.4</v>
+      </c>
+      <c r="AJ71" s="24">
+        <f>AVERAGE(Y71:AH71)</f>
+        <v>82.123333333333335</v>
+      </c>
+    </row>
+    <row r="72" spans="4:36" x14ac:dyDescent="0.25">
       <c r="D72" s="13">
         <v>0.99</v>
       </c>
@@ -1424,8 +1538,45 @@
       <c r="M72" s="1" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="73" spans="4:13" x14ac:dyDescent="0.25">
+      <c r="Y72">
+        <v>94.9</v>
+      </c>
+      <c r="Z72">
+        <v>97.2</v>
+      </c>
+      <c r="AB72">
+        <v>95.7</v>
+      </c>
+      <c r="AC72">
+        <f>AC71</f>
+        <v>99.6</v>
+      </c>
+      <c r="AD72">
+        <f t="shared" ref="AD72:AH72" si="0">AD71</f>
+        <v>95.08</v>
+      </c>
+      <c r="AE72">
+        <f t="shared" si="0"/>
+        <v>97.4</v>
+      </c>
+      <c r="AF72">
+        <f t="shared" si="0"/>
+        <v>63.76</v>
+      </c>
+      <c r="AG72">
+        <f t="shared" si="0"/>
+        <v>10.57</v>
+      </c>
+      <c r="AH72">
+        <f t="shared" si="0"/>
+        <v>99.4</v>
+      </c>
+      <c r="AJ72" s="24">
+        <f t="shared" ref="AJ72:AJ74" si="1">AVERAGE(Y72:AH72)</f>
+        <v>83.734444444444449</v>
+      </c>
+    </row>
+    <row r="73" spans="4:36" x14ac:dyDescent="0.25">
       <c r="D73" s="13">
         <v>0.5</v>
       </c>
@@ -1441,8 +1592,45 @@
       <c r="M73" s="1" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="74" spans="4:13" x14ac:dyDescent="0.25">
+      <c r="Y73">
+        <v>86.5</v>
+      </c>
+      <c r="Z73">
+        <v>96.2</v>
+      </c>
+      <c r="AB73">
+        <v>82.1</v>
+      </c>
+      <c r="AC73">
+        <f t="shared" ref="AC73:AC74" si="2">AC72</f>
+        <v>99.6</v>
+      </c>
+      <c r="AD73">
+        <f t="shared" ref="AD73:AD74" si="3">AD72</f>
+        <v>95.08</v>
+      </c>
+      <c r="AE73">
+        <f t="shared" ref="AE73:AE74" si="4">AE72</f>
+        <v>97.4</v>
+      </c>
+      <c r="AF73">
+        <f t="shared" ref="AF73:AF74" si="5">AF72</f>
+        <v>63.76</v>
+      </c>
+      <c r="AG73">
+        <f t="shared" ref="AG73:AG74" si="6">AG72</f>
+        <v>10.57</v>
+      </c>
+      <c r="AH73">
+        <f t="shared" ref="AH73:AH74" si="7">AH72</f>
+        <v>99.4</v>
+      </c>
+      <c r="AJ73" s="24">
+        <f t="shared" si="1"/>
+        <v>81.178888888888892</v>
+      </c>
+    </row>
+    <row r="74" spans="4:36" x14ac:dyDescent="0.25">
       <c r="D74" s="13">
         <v>1</v>
       </c>
@@ -1457,6 +1645,48 @@
       </c>
       <c r="M74" s="1" t="s">
         <v>69</v>
+      </c>
+      <c r="Y74">
+        <v>94.5</v>
+      </c>
+      <c r="Z74">
+        <v>97.2</v>
+      </c>
+      <c r="AB74">
+        <v>92.6</v>
+      </c>
+      <c r="AC74">
+        <f t="shared" si="2"/>
+        <v>99.6</v>
+      </c>
+      <c r="AD74">
+        <f t="shared" si="3"/>
+        <v>95.08</v>
+      </c>
+      <c r="AE74">
+        <f t="shared" si="4"/>
+        <v>97.4</v>
+      </c>
+      <c r="AF74">
+        <f t="shared" si="5"/>
+        <v>63.76</v>
+      </c>
+      <c r="AG74">
+        <f t="shared" si="6"/>
+        <v>10.57</v>
+      </c>
+      <c r="AH74">
+        <f t="shared" si="7"/>
+        <v>99.4</v>
+      </c>
+      <c r="AJ74" s="24">
+        <f t="shared" si="1"/>
+        <v>83.345555555555563</v>
+      </c>
+    </row>
+    <row r="75" spans="4:36" x14ac:dyDescent="0.25">
+      <c r="E75" s="23" t="s">
+        <v>78</v>
       </c>
     </row>
     <row r="84" spans="13:13" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Debugging resetAll to moving average Added results
</commit_message>
<xml_diff>
--- a/matlab_analysis/Results.xlsx
+++ b/matlab_analysis/Results.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="95">
   <si>
     <t>conf</t>
   </si>
@@ -235,25 +235,70 @@
     <t>UCB_C</t>
   </si>
   <si>
-    <t>case7</t>
-  </si>
-  <si>
-    <t>case8</t>
-  </si>
-  <si>
-    <t>case9</t>
-  </si>
-  <si>
-    <t>case10</t>
-  </si>
-  <si>
     <t>avg</t>
   </si>
   <si>
     <t>min 0.5</t>
   </si>
   <si>
-    <t>cases</t>
+    <t>all cases best</t>
+  </si>
+  <si>
+    <t>%%%%--- USE first_data_column = 2 FROM HERE ON !!!! ---%%%%</t>
+  </si>
+  <si>
+    <t>experiment_filenames{61}   = 'Reprint___2014_10_21_UCBT_2parms_resetSingle___2014_10_21_01_19_20';</t>
+  </si>
+  <si>
+    <t>CP_min</t>
+  </si>
+  <si>
+    <t>experiment_filenames{60}   = 'Reprint___2014_10_21_UCBT_4parms_resetSingle___2014_10_21_00_30_42';</t>
+  </si>
+  <si>
+    <t>experiment_filenames{62}   = 'Reprint___2014_10_21_Or1_UCBT_3parms_resetSingle___2014_10_20_13_19_04';</t>
+  </si>
+  <si>
+    <t>experiment_filenames{63}   = 'Reprint___2014_10_21_T3_Or0_Egre_CPthr_resetCut___2014_10_21_01_19_20';</t>
+  </si>
+  <si>
+    <t>experiment_filenames{64}   = 'Reprint___2014_10_21_T3_Or0_Egre_CPthr_resetMA___2014_10_21_01_19_20';</t>
+  </si>
+  <si>
+    <t>experiment_filenames{65}   = 'Reprint___2014_10_21_T3_Or0_Egre_CPthr_resetSingle___2014_10_21_01_19_20';</t>
+  </si>
+  <si>
+    <t>experiment_filenames{66}   = 'Reprint___2014_10_21_T3_Or0_Egre_CPthr_resetZero___2014_10_21_01_19_20';</t>
+  </si>
+  <si>
+    <t>experiment_filenames{67}   = 'Reprint___2014_10_21_T3_Or0_UCB1_CPthr_resetCut___2014_10_21_01_19_20';</t>
+  </si>
+  <si>
+    <t>experiment_filenames{68}   = 'Reprint___2014_10_21_T3_Or0_UCB1_CPthr_resetMA___2014_10_21_01_19_20';</t>
+  </si>
+  <si>
+    <t>experiment_filenames{69}   = 'Reprint___2014_10_21_T3_Or0_UCB1_CPthr_resetSingle___2014_10_21_01_19_21';</t>
+  </si>
+  <si>
+    <t>experiment_filenames{70}   = 'Reprint___2014_10_21_T3_Or0_UCB1_CPthr_resetZero___2014_10_21_01_19_20';</t>
+  </si>
+  <si>
+    <t>experiment_filenames{71}   = 'Reprint___2014_10_21_T3_Or0_UCBT_CPthr_resetCut___2014_10_21_01_19_21';</t>
+  </si>
+  <si>
+    <t>experiment_filenames{72}   = 'Reprint___2014_10_21_T3_Or0_UCBT_CPthr_resetMA___2014_10_21_01_19_21';</t>
+  </si>
+  <si>
+    <t>experiment_filenames{73}   = 'Reprint___2014_10_21_T3_Or0_UCBT_CPthr_resetSingle___2014_10_21_01_19_21';</t>
+  </si>
+  <si>
+    <t>experiment_filenames{74}   = 'Reprint___2014_10_21_T3_Or0_UCBT_CPthr_resetZero___2014_10_21_10_32_18';</t>
+  </si>
+  <si>
+    <t>0.65 or 5.50</t>
+  </si>
+  <si>
+    <t>best scores by cases</t>
   </si>
 </sst>
 </file>
@@ -264,7 +309,7 @@
     <numFmt numFmtId="164" formatCode="0.0"/>
     <numFmt numFmtId="165" formatCode="0.000"/>
   </numFmts>
-  <fonts count="14" x14ac:knownFonts="1">
+  <fonts count="15" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -378,6 +423,12 @@
       <charset val="238"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -399,7 +450,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -447,6 +498,8 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="165" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -753,8 +806,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AJ422"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="X51" workbookViewId="0">
-      <selection activeCell="AI80" sqref="AI80"/>
+    <sheetView tabSelected="1" topLeftCell="N63" workbookViewId="0">
+      <selection activeCell="AK90" sqref="AK90"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -991,12 +1044,12 @@
         <v>37</v>
       </c>
     </row>
-    <row r="33" spans="5:13" x14ac:dyDescent="0.25">
+    <row r="33" spans="5:36" x14ac:dyDescent="0.25">
       <c r="M33" s="7" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="34" spans="5:13" x14ac:dyDescent="0.25">
+    <row r="34" spans="5:36" x14ac:dyDescent="0.25">
       <c r="E34" s="13">
         <v>0.34</v>
       </c>
@@ -1007,7 +1060,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="35" spans="5:13" x14ac:dyDescent="0.25">
+    <row r="35" spans="5:36" x14ac:dyDescent="0.25">
       <c r="E35" s="13">
         <v>1.1000000000000001</v>
       </c>
@@ -1018,7 +1071,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="36" spans="5:13" x14ac:dyDescent="0.25">
+    <row r="36" spans="5:36" x14ac:dyDescent="0.25">
       <c r="E36" s="13">
         <v>5.0000000000000001E-3</v>
       </c>
@@ -1029,12 +1082,12 @@
         <v>38</v>
       </c>
     </row>
-    <row r="37" spans="5:13" x14ac:dyDescent="0.25">
+    <row r="37" spans="5:36" x14ac:dyDescent="0.25">
       <c r="M37" s="7" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="38" spans="5:13" x14ac:dyDescent="0.25">
+    <row r="38" spans="5:36" x14ac:dyDescent="0.25">
       <c r="E38" s="13">
         <v>8.5000000000000006E-2</v>
       </c>
@@ -1045,7 +1098,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="39" spans="5:13" x14ac:dyDescent="0.25">
+    <row r="39" spans="5:36" x14ac:dyDescent="0.25">
       <c r="E39" s="13">
         <v>0.23</v>
       </c>
@@ -1055,11 +1108,29 @@
       <c r="M39" s="7" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="40" spans="5:13" x14ac:dyDescent="0.25">
+      <c r="Y39" s="22"/>
+      <c r="AC39" s="22"/>
+      <c r="AD39" s="22"/>
+      <c r="AE39" s="22"/>
+      <c r="AF39" s="22"/>
+      <c r="AG39" s="22"/>
+      <c r="AH39" s="22"/>
+    </row>
+    <row r="40" spans="5:36" x14ac:dyDescent="0.25">
       <c r="M40" s="7"/>
-    </row>
-    <row r="41" spans="5:13" x14ac:dyDescent="0.25">
+      <c r="Y40" s="22"/>
+      <c r="Z40" s="22"/>
+      <c r="AA40" s="22"/>
+      <c r="AB40" s="22"/>
+      <c r="AC40" s="22"/>
+      <c r="AD40" s="22"/>
+      <c r="AE40" s="22"/>
+      <c r="AF40" s="22"/>
+      <c r="AG40" s="22"/>
+      <c r="AH40" s="22"/>
+      <c r="AJ40" s="22"/>
+    </row>
+    <row r="41" spans="5:36" x14ac:dyDescent="0.25">
       <c r="E41" s="13">
         <v>0.14000000000000001</v>
       </c>
@@ -1069,8 +1140,19 @@
       <c r="M41" s="7" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="42" spans="5:13" x14ac:dyDescent="0.25">
+      <c r="Y41" s="26"/>
+      <c r="Z41" s="26"/>
+      <c r="AA41" s="26"/>
+      <c r="AB41" s="26"/>
+      <c r="AC41" s="26"/>
+      <c r="AD41" s="26"/>
+      <c r="AE41" s="26"/>
+      <c r="AF41" s="26"/>
+      <c r="AG41" s="26"/>
+      <c r="AH41" s="26"/>
+      <c r="AJ41" s="24"/>
+    </row>
+    <row r="42" spans="5:36" x14ac:dyDescent="0.25">
       <c r="E42" s="13">
         <v>1E-3</v>
       </c>
@@ -1082,7 +1164,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="43" spans="5:13" x14ac:dyDescent="0.25">
+    <row r="43" spans="5:36" x14ac:dyDescent="0.25">
       <c r="E43" s="13">
         <v>0.24</v>
       </c>
@@ -1097,7 +1179,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="44" spans="5:13" x14ac:dyDescent="0.25">
+    <row r="44" spans="5:36" x14ac:dyDescent="0.25">
       <c r="E44" s="13">
         <v>0.77</v>
       </c>
@@ -1111,7 +1193,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="45" spans="5:13" x14ac:dyDescent="0.25">
+    <row r="45" spans="5:36" x14ac:dyDescent="0.25">
       <c r="E45" s="13">
         <v>0.02</v>
       </c>
@@ -1122,7 +1204,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="46" spans="5:13" x14ac:dyDescent="0.25">
+    <row r="46" spans="5:36" x14ac:dyDescent="0.25">
       <c r="E46" s="13">
         <v>3.0000000000000001E-3</v>
       </c>
@@ -1133,7 +1215,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="47" spans="5:13" x14ac:dyDescent="0.25">
+    <row r="47" spans="5:36" x14ac:dyDescent="0.25">
       <c r="E47" s="13">
         <v>5.8999999999999997E-2</v>
       </c>
@@ -1147,7 +1229,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="48" spans="5:13" x14ac:dyDescent="0.25">
+    <row r="48" spans="5:36" x14ac:dyDescent="0.25">
       <c r="E48" s="13">
         <v>0.16600000000000001</v>
       </c>
@@ -1345,7 +1427,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="65" spans="4:36" x14ac:dyDescent="0.25">
+    <row r="65" spans="2:36" x14ac:dyDescent="0.25">
       <c r="D65" s="19" t="s">
         <v>70</v>
       </c>
@@ -1353,7 +1435,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="66" spans="4:36" x14ac:dyDescent="0.25">
+    <row r="66" spans="2:36" x14ac:dyDescent="0.25">
       <c r="D66" s="13">
         <v>1.8</v>
       </c>
@@ -1371,7 +1453,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="67" spans="4:36" x14ac:dyDescent="0.25">
+    <row r="67" spans="2:36" x14ac:dyDescent="0.25">
       <c r="D67" s="13">
         <v>2.2999999999999998</v>
       </c>
@@ -1389,7 +1471,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="68" spans="4:36" x14ac:dyDescent="0.25">
+    <row r="68" spans="2:36" x14ac:dyDescent="0.25">
       <c r="D68" s="13">
         <v>2.2000000000000002</v>
       </c>
@@ -1407,7 +1489,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="69" spans="4:36" x14ac:dyDescent="0.25">
+    <row r="69" spans="2:36" x14ac:dyDescent="0.25">
       <c r="D69" s="13">
         <v>0.5</v>
       </c>
@@ -1423,34 +1505,38 @@
       <c r="M69" s="7" t="s">
         <v>65</v>
       </c>
-      <c r="AC69" s="22" t="s">
-        <v>79</v>
-      </c>
+      <c r="Y69" s="22" t="s">
+        <v>94</v>
+      </c>
+      <c r="AC69" s="22"/>
       <c r="AD69" s="22"/>
       <c r="AE69" s="22"/>
       <c r="AF69" s="22"/>
       <c r="AG69" s="22"/>
       <c r="AH69" s="22"/>
     </row>
-    <row r="70" spans="4:36" x14ac:dyDescent="0.25">
+    <row r="70" spans="2:36" x14ac:dyDescent="0.25">
       <c r="D70" s="19" t="s">
         <v>71</v>
       </c>
       <c r="E70" s="19" t="s">
         <v>70</v>
       </c>
+      <c r="J70" s="5" t="s">
+        <v>75</v>
+      </c>
       <c r="M70" s="7"/>
-      <c r="Y70" s="22" t="s">
-        <v>73</v>
-      </c>
-      <c r="Z70" s="22" t="s">
-        <v>74</v>
-      </c>
-      <c r="AA70" s="22" t="s">
-        <v>75</v>
-      </c>
-      <c r="AB70" s="22" t="s">
-        <v>76</v>
+      <c r="Y70" s="22">
+        <v>7</v>
+      </c>
+      <c r="Z70" s="22">
+        <v>8</v>
+      </c>
+      <c r="AA70" s="22">
+        <v>9</v>
+      </c>
+      <c r="AB70" s="22">
+        <v>10</v>
       </c>
       <c r="AC70" s="22">
         <v>1</v>
@@ -1471,10 +1557,10 @@
         <v>6</v>
       </c>
       <c r="AJ70" s="22" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="71" spans="4:36" x14ac:dyDescent="0.25">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="71" spans="2:36" x14ac:dyDescent="0.25">
       <c r="D71" s="13">
         <v>0.65500000000000003</v>
       </c>
@@ -1487,14 +1573,21 @@
       <c r="H71" s="20">
         <v>0</v>
       </c>
+      <c r="J71" s="11">
+        <f>AJ71</f>
+        <v>83.911000000000001</v>
+      </c>
       <c r="M71" s="1" t="s">
         <v>66</v>
       </c>
       <c r="Y71">
         <v>93.3</v>
       </c>
-      <c r="Z71">
+      <c r="Z71" s="25">
         <v>97.9</v>
+      </c>
+      <c r="AA71">
+        <v>100</v>
       </c>
       <c r="AB71">
         <v>82.1</v>
@@ -1519,10 +1612,10 @@
       </c>
       <c r="AJ71" s="24">
         <f>AVERAGE(Y71:AH71)</f>
-        <v>82.123333333333335</v>
-      </c>
-    </row>
-    <row r="72" spans="4:36" x14ac:dyDescent="0.25">
+        <v>83.911000000000001</v>
+      </c>
+    </row>
+    <row r="72" spans="2:36" x14ac:dyDescent="0.25">
       <c r="D72" s="13">
         <v>0.99</v>
       </c>
@@ -1535,24 +1628,31 @@
       <c r="H72" s="20">
         <v>0</v>
       </c>
+      <c r="J72" s="11">
+        <f>AJ72</f>
+        <v>85.361000000000004</v>
+      </c>
       <c r="M72" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="Y72">
+      <c r="Y72" s="25">
         <v>94.9</v>
       </c>
       <c r="Z72">
         <v>97.2</v>
       </c>
-      <c r="AB72">
+      <c r="AA72">
+        <v>100</v>
+      </c>
+      <c r="AB72" s="25">
         <v>95.7</v>
       </c>
       <c r="AC72">
-        <f>AC71</f>
+        <f t="shared" ref="AC72:AH74" si="0">AC71</f>
         <v>99.6</v>
       </c>
       <c r="AD72">
-        <f t="shared" ref="AD72:AH72" si="0">AD71</f>
+        <f t="shared" si="0"/>
         <v>95.08</v>
       </c>
       <c r="AE72">
@@ -1572,11 +1672,11 @@
         <v>99.4</v>
       </c>
       <c r="AJ72" s="24">
-        <f t="shared" ref="AJ72:AJ74" si="1">AVERAGE(Y72:AH72)</f>
-        <v>83.734444444444449</v>
-      </c>
-    </row>
-    <row r="73" spans="4:36" x14ac:dyDescent="0.25">
+        <f>AVERAGE(Y72:AH72)</f>
+        <v>85.361000000000004</v>
+      </c>
+    </row>
+    <row r="73" spans="2:36" x14ac:dyDescent="0.25">
       <c r="D73" s="13">
         <v>0.5</v>
       </c>
@@ -1589,6 +1689,10 @@
       <c r="H73" s="20">
         <v>0</v>
       </c>
+      <c r="J73" s="11">
+        <f>AJ73</f>
+        <v>83.061000000000007</v>
+      </c>
       <c r="M73" s="1" t="s">
         <v>68</v>
       </c>
@@ -1598,39 +1702,42 @@
       <c r="Z73">
         <v>96.2</v>
       </c>
+      <c r="AA73">
+        <v>100</v>
+      </c>
       <c r="AB73">
         <v>82.1</v>
       </c>
       <c r="AC73">
-        <f t="shared" ref="AC73:AC74" si="2">AC72</f>
+        <f t="shared" si="0"/>
         <v>99.6</v>
       </c>
       <c r="AD73">
-        <f t="shared" ref="AD73:AD74" si="3">AD72</f>
+        <f t="shared" si="0"/>
         <v>95.08</v>
       </c>
       <c r="AE73">
-        <f t="shared" ref="AE73:AE74" si="4">AE72</f>
+        <f t="shared" si="0"/>
         <v>97.4</v>
       </c>
       <c r="AF73">
-        <f t="shared" ref="AF73:AF74" si="5">AF72</f>
+        <f t="shared" si="0"/>
         <v>63.76</v>
       </c>
       <c r="AG73">
-        <f t="shared" ref="AG73:AG74" si="6">AG72</f>
+        <f t="shared" si="0"/>
         <v>10.57</v>
       </c>
       <c r="AH73">
-        <f t="shared" ref="AH73:AH74" si="7">AH72</f>
+        <f t="shared" si="0"/>
         <v>99.4</v>
       </c>
       <c r="AJ73" s="24">
-        <f t="shared" si="1"/>
-        <v>81.178888888888892</v>
-      </c>
-    </row>
-    <row r="74" spans="4:36" x14ac:dyDescent="0.25">
+        <f>AVERAGE(Y73:AH73)</f>
+        <v>83.061000000000007</v>
+      </c>
+    </row>
+    <row r="74" spans="2:36" x14ac:dyDescent="0.25">
       <c r="D74" s="13">
         <v>1</v>
       </c>
@@ -1643,6 +1750,10 @@
       <c r="H74" s="20">
         <v>0</v>
       </c>
+      <c r="J74" s="11">
+        <f>AJ74</f>
+        <v>85.010999999999996</v>
+      </c>
       <c r="M74" s="1" t="s">
         <v>69</v>
       </c>
@@ -1652,48 +1763,566 @@
       <c r="Z74">
         <v>97.2</v>
       </c>
+      <c r="AA74">
+        <v>100</v>
+      </c>
       <c r="AB74">
         <v>92.6</v>
       </c>
       <c r="AC74">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>99.6</v>
       </c>
       <c r="AD74">
+        <f t="shared" si="0"/>
+        <v>95.08</v>
+      </c>
+      <c r="AE74">
+        <f t="shared" si="0"/>
+        <v>97.4</v>
+      </c>
+      <c r="AF74">
+        <f t="shared" si="0"/>
+        <v>63.76</v>
+      </c>
+      <c r="AG74">
+        <f t="shared" si="0"/>
+        <v>10.57</v>
+      </c>
+      <c r="AH74">
+        <f t="shared" si="0"/>
+        <v>99.4</v>
+      </c>
+      <c r="AJ74" s="24">
+        <f>AVERAGE(Y74:AH74)</f>
+        <v>85.010999999999996</v>
+      </c>
+    </row>
+    <row r="75" spans="2:36" x14ac:dyDescent="0.25">
+      <c r="E75" s="23" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="76" spans="2:36" x14ac:dyDescent="0.25">
+      <c r="M76" s="2" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="77" spans="2:36" x14ac:dyDescent="0.25">
+      <c r="B77" s="19" t="s">
+        <v>78</v>
+      </c>
+      <c r="C77" s="19" t="s">
+        <v>71</v>
+      </c>
+      <c r="D77" s="19" t="s">
+        <v>70</v>
+      </c>
+      <c r="E77" s="19" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="78" spans="2:36" x14ac:dyDescent="0.25">
+      <c r="B78" s="13">
+        <v>30</v>
+      </c>
+      <c r="C78" s="13">
+        <v>0.9</v>
+      </c>
+      <c r="D78" s="13">
+        <v>1.6</v>
+      </c>
+      <c r="E78" s="13">
+        <v>0.8</v>
+      </c>
+      <c r="G78" s="11">
+        <v>65.5</v>
+      </c>
+      <c r="H78" s="20">
+        <v>0.6</v>
+      </c>
+      <c r="M78" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="Y78">
+        <v>79.7</v>
+      </c>
+      <c r="Z78">
+        <v>88.7</v>
+      </c>
+      <c r="AA78">
+        <v>103.1</v>
+      </c>
+      <c r="AB78">
+        <v>74.5</v>
+      </c>
+      <c r="AC78">
+        <v>114.4</v>
+      </c>
+      <c r="AD78">
+        <v>106.5</v>
+      </c>
+      <c r="AE78">
+        <v>103</v>
+      </c>
+      <c r="AF78">
+        <v>81.2</v>
+      </c>
+      <c r="AG78">
+        <v>55.6</v>
+      </c>
+      <c r="AH78">
+        <v>93</v>
+      </c>
+      <c r="AJ78">
+        <f>AVERAGE(Y78:AH78)</f>
+        <v>89.97</v>
+      </c>
+    </row>
+    <row r="79" spans="2:36" x14ac:dyDescent="0.25">
+      <c r="B79" s="16">
+        <v>230</v>
+      </c>
+      <c r="C79" s="13">
+        <v>1</v>
+      </c>
+      <c r="D79" s="16">
+        <v>0.95</v>
+      </c>
+      <c r="E79" s="13">
+        <v>0.77</v>
+      </c>
+      <c r="G79" s="11">
+        <v>63.1</v>
+      </c>
+      <c r="H79" s="20">
+        <v>1.2</v>
+      </c>
+      <c r="M79" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="Y79">
+        <v>77.7</v>
+      </c>
+      <c r="Z79">
+        <v>86</v>
+      </c>
+      <c r="AA79">
+        <v>100.3</v>
+      </c>
+      <c r="AB79">
+        <v>68.3</v>
+      </c>
+      <c r="AC79">
+        <v>111</v>
+      </c>
+      <c r="AD79">
+        <v>105</v>
+      </c>
+      <c r="AE79">
+        <v>92.8</v>
+      </c>
+      <c r="AF79">
+        <v>48.7</v>
+      </c>
+      <c r="AG79">
+        <v>37.799999999999997</v>
+      </c>
+      <c r="AH79">
+        <v>82.2</v>
+      </c>
+      <c r="AJ79">
+        <f>AVERAGE(Y79:AH79)</f>
+        <v>80.97999999999999</v>
+      </c>
+    </row>
+    <row r="80" spans="2:36" x14ac:dyDescent="0.25">
+      <c r="B80" s="13">
+        <v>20</v>
+      </c>
+      <c r="C80" s="13">
+        <v>1</v>
+      </c>
+      <c r="D80" s="13">
+        <v>1</v>
+      </c>
+      <c r="G80" s="11">
+        <v>96.1</v>
+      </c>
+      <c r="H80" s="20">
+        <v>0.04</v>
+      </c>
+      <c r="M80" s="1" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="81" spans="4:36" x14ac:dyDescent="0.25">
+      <c r="D81" s="19" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="82" spans="4:36" x14ac:dyDescent="0.25">
+      <c r="D82" s="13">
+        <v>3.7</v>
+      </c>
+      <c r="G82" s="11">
+        <v>61.4</v>
+      </c>
+      <c r="H82" s="20">
+        <v>1.4</v>
+      </c>
+      <c r="M82" s="1" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="83" spans="4:36" x14ac:dyDescent="0.25">
+      <c r="M83" s="1" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="84" spans="4:36" x14ac:dyDescent="0.25">
+      <c r="D84" s="13">
+        <v>3.1</v>
+      </c>
+      <c r="G84" s="11">
+        <v>60.1</v>
+      </c>
+      <c r="H84" s="20">
+        <v>1.6</v>
+      </c>
+      <c r="M84" s="7" t="s">
+        <v>83</v>
+      </c>
+      <c r="Y84">
+        <v>60.7</v>
+      </c>
+      <c r="Z84">
+        <v>69.900000000000006</v>
+      </c>
+      <c r="AA84">
+        <v>83</v>
+      </c>
+      <c r="AB84">
+        <v>60.2</v>
+      </c>
+      <c r="AC84">
+        <v>92.5</v>
+      </c>
+      <c r="AD84">
+        <v>105</v>
+      </c>
+      <c r="AE84">
+        <v>97.4</v>
+      </c>
+      <c r="AF84">
+        <v>69.2</v>
+      </c>
+      <c r="AG84">
+        <v>59.7</v>
+      </c>
+      <c r="AH84">
+        <v>76.400000000000006</v>
+      </c>
+      <c r="AJ84">
+        <f t="shared" ref="AJ84" si="1">AVERAGE(Y84:AH84)</f>
+        <v>77.400000000000006</v>
+      </c>
+    </row>
+    <row r="85" spans="4:36" x14ac:dyDescent="0.25">
+      <c r="D85" s="13">
+        <v>3.8</v>
+      </c>
+      <c r="G85" s="11">
+        <v>58</v>
+      </c>
+      <c r="H85" s="20">
+        <v>0.6</v>
+      </c>
+      <c r="M85" s="1" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="87" spans="4:36" x14ac:dyDescent="0.25">
+      <c r="D87" s="13">
+        <v>6</v>
+      </c>
+      <c r="G87" s="11">
+        <v>59.3</v>
+      </c>
+      <c r="H87" s="20">
+        <v>0.9</v>
+      </c>
+      <c r="M87" s="1" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="88" spans="4:36" x14ac:dyDescent="0.25">
+      <c r="D88" s="13">
+        <v>7</v>
+      </c>
+      <c r="G88" s="11">
+        <v>57.8</v>
+      </c>
+      <c r="H88" s="20">
+        <v>1</v>
+      </c>
+      <c r="M88" s="1" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="89" spans="4:36" x14ac:dyDescent="0.25">
+      <c r="D89" s="13">
+        <v>2.5</v>
+      </c>
+      <c r="G89" s="11">
+        <v>63.7</v>
+      </c>
+      <c r="H89" s="20">
+        <v>0.7</v>
+      </c>
+      <c r="M89" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="Y89">
+        <v>73.400000000000006</v>
+      </c>
+      <c r="Z89">
+        <v>84.7</v>
+      </c>
+      <c r="AA89">
+        <v>99.9</v>
+      </c>
+      <c r="AB89">
+        <v>69.099999999999994</v>
+      </c>
+      <c r="AC89">
+        <v>110.9</v>
+      </c>
+      <c r="AD89">
+        <v>96.7</v>
+      </c>
+      <c r="AE89">
+        <v>97.8</v>
+      </c>
+      <c r="AF89">
+        <v>64.900000000000006</v>
+      </c>
+      <c r="AG89">
+        <v>49.72</v>
+      </c>
+      <c r="AH89">
+        <v>86.9</v>
+      </c>
+      <c r="AJ89">
+        <f t="shared" ref="AJ89" si="2">AVERAGE(Y89:AH89)</f>
+        <v>83.402000000000001</v>
+      </c>
+    </row>
+    <row r="90" spans="4:36" x14ac:dyDescent="0.25">
+      <c r="D90" s="13">
+        <v>6</v>
+      </c>
+      <c r="G90" s="11">
+        <v>58.47</v>
+      </c>
+      <c r="H90" s="20">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="M90" s="1" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="92" spans="4:36" x14ac:dyDescent="0.25">
+      <c r="D92" s="13">
+        <v>6</v>
+      </c>
+      <c r="G92" s="11">
+        <v>59.02</v>
+      </c>
+      <c r="H92" s="20">
+        <v>1.3</v>
+      </c>
+      <c r="M92" s="7" t="s">
+        <v>89</v>
+      </c>
+      <c r="Y92">
+        <v>69.5</v>
+      </c>
+      <c r="Z92">
+        <v>83.9</v>
+      </c>
+      <c r="AA92">
+        <v>78.599999999999994</v>
+      </c>
+      <c r="AB92">
+        <v>42.7</v>
+      </c>
+      <c r="AC92">
+        <v>108.4</v>
+      </c>
+      <c r="AD92">
+        <v>93.4</v>
+      </c>
+      <c r="AE92">
+        <v>94.9</v>
+      </c>
+      <c r="AF92">
+        <v>40.799999999999997</v>
+      </c>
+      <c r="AG92">
+        <v>63.6</v>
+      </c>
+      <c r="AH92">
+        <v>85.8</v>
+      </c>
+      <c r="AJ92">
+        <f t="shared" ref="AJ92:AJ94" si="3">AVERAGE(Y92:AH92)</f>
+        <v>76.16</v>
+      </c>
+    </row>
+    <row r="93" spans="4:36" x14ac:dyDescent="0.25">
+      <c r="D93" s="13">
+        <v>5</v>
+      </c>
+      <c r="G93" s="11">
+        <v>57.7</v>
+      </c>
+      <c r="H93" s="20">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="M93" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="Y93">
+        <v>67.5</v>
+      </c>
+      <c r="Z93">
+        <v>83.8</v>
+      </c>
+      <c r="AA93">
+        <v>82.5</v>
+      </c>
+      <c r="AB93">
+        <v>41.8</v>
+      </c>
+      <c r="AC93">
+        <v>107.3</v>
+      </c>
+      <c r="AD93">
+        <v>86.2</v>
+      </c>
+      <c r="AE93">
+        <v>97.5</v>
+      </c>
+      <c r="AF93">
+        <v>37.200000000000003</v>
+      </c>
+      <c r="AG93">
+        <v>46.1</v>
+      </c>
+      <c r="AH93">
+        <v>89.6</v>
+      </c>
+      <c r="AJ93">
         <f t="shared" si="3"/>
-        <v>95.08</v>
-      </c>
-      <c r="AE74">
-        <f t="shared" si="4"/>
-        <v>97.4</v>
-      </c>
-      <c r="AF74">
-        <f t="shared" si="5"/>
-        <v>63.76</v>
-      </c>
-      <c r="AG74">
-        <f t="shared" si="6"/>
-        <v>10.57</v>
-      </c>
-      <c r="AH74">
-        <f t="shared" si="7"/>
-        <v>99.4</v>
-      </c>
-      <c r="AJ74" s="24">
-        <f t="shared" si="1"/>
-        <v>83.345555555555563</v>
-      </c>
-    </row>
-    <row r="75" spans="4:36" x14ac:dyDescent="0.25">
-      <c r="E75" s="23" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="84" spans="13:13" x14ac:dyDescent="0.25">
-      <c r="M84" s="2"/>
-    </row>
-    <row r="92" spans="13:13" x14ac:dyDescent="0.25">
-      <c r="M92" s="2"/>
+        <v>73.950000000000017</v>
+      </c>
+    </row>
+    <row r="94" spans="4:36" x14ac:dyDescent="0.25">
+      <c r="D94" s="13" t="s">
+        <v>93</v>
+      </c>
+      <c r="G94" s="11">
+        <v>67.39</v>
+      </c>
+      <c r="H94" s="20">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="M94" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="Y94">
+        <v>68.599999999999994</v>
+      </c>
+      <c r="Z94">
+        <v>86.5</v>
+      </c>
+      <c r="AA94">
+        <v>99.59</v>
+      </c>
+      <c r="AB94">
+        <v>62.7</v>
+      </c>
+      <c r="AC94">
+        <v>108</v>
+      </c>
+      <c r="AD94">
+        <v>95.1</v>
+      </c>
+      <c r="AE94">
+        <v>91.9</v>
+      </c>
+      <c r="AF94">
+        <v>45.2</v>
+      </c>
+      <c r="AG94">
+        <v>50.3</v>
+      </c>
+      <c r="AH94">
+        <v>81.900000000000006</v>
+      </c>
+      <c r="AJ94">
+        <f t="shared" si="3"/>
+        <v>78.978999999999999</v>
+      </c>
+    </row>
+    <row r="95" spans="4:36" x14ac:dyDescent="0.25">
+      <c r="D95" s="13">
+        <v>6</v>
+      </c>
+      <c r="G95" s="11">
+        <v>56.5</v>
+      </c>
+      <c r="H95" s="20">
+        <v>1.5</v>
+      </c>
+      <c r="M95" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="Y95">
+        <v>66.8</v>
+      </c>
+      <c r="Z95">
+        <v>85.3</v>
+      </c>
+      <c r="AA95">
+        <v>77.3</v>
+      </c>
+      <c r="AB95">
+        <v>38.9</v>
+      </c>
+      <c r="AC95">
+        <v>102</v>
+      </c>
+      <c r="AD95">
+        <v>78.900000000000006</v>
+      </c>
+      <c r="AE95">
+        <v>88.8</v>
+      </c>
+      <c r="AF95">
+        <v>39.5</v>
+      </c>
+      <c r="AG95">
+        <v>57.8</v>
+      </c>
+      <c r="AH95">
+        <v>85.9</v>
+      </c>
+      <c r="AJ95">
+        <f>AVERAGE(Y95:AH95)</f>
+        <v>72.119999999999976</v>
+      </c>
     </row>
     <row r="101" spans="13:13" x14ac:dyDescent="0.25">
       <c r="M101" s="2"/>
@@ -1948,6 +2577,138 @@
       <c r="M422" s="2"/>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="Y78:Y95">
+    <cfRule type="colorScale" priority="11">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="Z78:Z95">
+    <cfRule type="colorScale" priority="10">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AA78:AA95">
+    <cfRule type="colorScale" priority="9">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AB78:AB95">
+    <cfRule type="colorScale" priority="8">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AC78:AC95">
+    <cfRule type="colorScale" priority="7">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AD78:AD95">
+    <cfRule type="colorScale" priority="6">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AE78:AE95">
+    <cfRule type="colorScale" priority="5">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AF78:AF95">
+    <cfRule type="colorScale" priority="4">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AG78:AG95">
+    <cfRule type="colorScale" priority="3">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AH78:AH95">
+    <cfRule type="colorScale" priority="2">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AJ78:AJ95">
+    <cfRule type="colorScale" priority="1">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
First paper draft and results
</commit_message>
<xml_diff>
--- a/matlab_analysis/Results.xlsx
+++ b/matlab_analysis/Results.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="105">
   <si>
     <t>conf</t>
   </si>
@@ -299,6 +299,36 @@
   </si>
   <si>
     <t>best scores by cases</t>
+  </si>
+  <si>
+    <t>%2014_10_21 no change point (redone with improved output)</t>
+  </si>
+  <si>
+    <t>experiment_filenames{75}   = 'Reprint___2014_10_21_noCPD_Egreedy_perStep10___2014_10_21_19_02_42';</t>
+  </si>
+  <si>
+    <t>experiment_filenames{76}   = 'Reprint___2014_10_21_noCPD_UCB1_perStep10___2014_10_21_19_04_47';</t>
+  </si>
+  <si>
+    <t>experiment_filenames{77}   = 'Reprint___2014_10_21_noCPD_UCBT_perStep10___2014_10_21_19_05_39';</t>
+  </si>
+  <si>
+    <t>%2014_10_21 experiments with more than 10 evaluations per sample</t>
+  </si>
+  <si>
+    <t>experiment_filenames{78}   = 'Reprint___2014_10_21_noCPD_Egreedy_perStep25___2014_10_21_19_03_05';</t>
+  </si>
+  <si>
+    <t>experiment_filenames{79}   = 'Reprint___2014_10_21_noCPD_UCB1_perStep25___2014_10_21_19_04_21';</t>
+  </si>
+  <si>
+    <t>experiment_filenames{80}   = 'Reprint___2014_10_21_noCPD_UCBT_perStep25___2014_10_21_19_06_24';</t>
+  </si>
+  <si>
+    <t>Epsilon or UCB_C</t>
+  </si>
+  <si>
+    <t>avgMax</t>
   </si>
 </sst>
 </file>
@@ -450,7 +480,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -500,6 +530,7 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -804,10 +835,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AJ422"/>
+  <dimension ref="A1:AK422"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F71" workbookViewId="0">
-      <selection activeCell="AE103" sqref="AE103"/>
+    <sheetView tabSelected="1" topLeftCell="Z61" workbookViewId="0">
+      <selection activeCell="AM80" sqref="AM80"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1427,7 +1458,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="65" spans="2:36" x14ac:dyDescent="0.25">
+    <row r="65" spans="2:37" x14ac:dyDescent="0.25">
       <c r="D65" s="19" t="s">
         <v>70</v>
       </c>
@@ -1435,7 +1466,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="66" spans="2:36" x14ac:dyDescent="0.25">
+    <row r="66" spans="2:37" x14ac:dyDescent="0.25">
       <c r="D66" s="13">
         <v>1.8</v>
       </c>
@@ -1453,7 +1484,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="67" spans="2:36" x14ac:dyDescent="0.25">
+    <row r="67" spans="2:37" x14ac:dyDescent="0.25">
       <c r="D67" s="13">
         <v>2.2999999999999998</v>
       </c>
@@ -1471,7 +1502,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="68" spans="2:36" x14ac:dyDescent="0.25">
+    <row r="68" spans="2:37" x14ac:dyDescent="0.25">
       <c r="D68" s="13">
         <v>2.2000000000000002</v>
       </c>
@@ -1489,7 +1520,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="69" spans="2:36" x14ac:dyDescent="0.25">
+    <row r="69" spans="2:37" x14ac:dyDescent="0.25">
       <c r="D69" s="13">
         <v>0.5</v>
       </c>
@@ -1515,7 +1546,7 @@
       <c r="AG69" s="22"/>
       <c r="AH69" s="22"/>
     </row>
-    <row r="70" spans="2:36" x14ac:dyDescent="0.25">
+    <row r="70" spans="2:37" x14ac:dyDescent="0.25">
       <c r="D70" s="19" t="s">
         <v>71</v>
       </c>
@@ -1556,11 +1587,14 @@
       <c r="AH70" s="22">
         <v>6</v>
       </c>
-      <c r="AJ70" s="22" t="s">
+      <c r="AJ70" s="27" t="s">
+        <v>104</v>
+      </c>
+      <c r="AK70" s="24" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="71" spans="2:36" x14ac:dyDescent="0.25">
+    <row r="71" spans="2:37" x14ac:dyDescent="0.25">
       <c r="D71" s="13">
         <v>0.65500000000000003</v>
       </c>
@@ -1614,8 +1648,12 @@
         <f>AVERAGE(Y71:AH71)</f>
         <v>83.911000000000001</v>
       </c>
-    </row>
-    <row r="72" spans="2:36" x14ac:dyDescent="0.25">
+      <c r="AK71" s="24">
+        <f>G71</f>
+        <v>83.4</v>
+      </c>
+    </row>
+    <row r="72" spans="2:37" x14ac:dyDescent="0.25">
       <c r="D72" s="13">
         <v>0.99</v>
       </c>
@@ -1675,8 +1713,12 @@
         <f>AVERAGE(Y72:AH72)</f>
         <v>85.361000000000004</v>
       </c>
-    </row>
-    <row r="73" spans="2:36" x14ac:dyDescent="0.25">
+      <c r="AK72" s="24">
+        <f t="shared" ref="AK72:AK95" si="1">G72</f>
+        <v>84.78</v>
+      </c>
+    </row>
+    <row r="73" spans="2:37" x14ac:dyDescent="0.25">
       <c r="D73" s="13">
         <v>0.5</v>
       </c>
@@ -1736,8 +1778,12 @@
         <f>AVERAGE(Y73:AH73)</f>
         <v>83.061000000000007</v>
       </c>
-    </row>
-    <row r="74" spans="2:36" x14ac:dyDescent="0.25">
+      <c r="AK73" s="24">
+        <f t="shared" si="1"/>
+        <v>82.67</v>
+      </c>
+    </row>
+    <row r="74" spans="2:37" x14ac:dyDescent="0.25">
       <c r="D74" s="13">
         <v>1</v>
       </c>
@@ -1797,18 +1843,26 @@
         <f>AVERAGE(Y74:AH74)</f>
         <v>85.010999999999996</v>
       </c>
-    </row>
-    <row r="75" spans="2:36" x14ac:dyDescent="0.25">
+      <c r="AK74" s="24">
+        <f t="shared" si="1"/>
+        <v>84.97</v>
+      </c>
+    </row>
+    <row r="75" spans="2:37" x14ac:dyDescent="0.25">
       <c r="E75" s="23" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="76" spans="2:36" x14ac:dyDescent="0.25">
+      <c r="AJ75" s="24"/>
+      <c r="AK75" s="24"/>
+    </row>
+    <row r="76" spans="2:37" x14ac:dyDescent="0.25">
       <c r="M76" s="2" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="77" spans="2:36" x14ac:dyDescent="0.25">
+      <c r="AJ76" s="24"/>
+      <c r="AK76" s="24"/>
+    </row>
+    <row r="77" spans="2:37" x14ac:dyDescent="0.25">
       <c r="B77" s="19" t="s">
         <v>78</v>
       </c>
@@ -1821,8 +1875,10 @@
       <c r="E77" s="19" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="78" spans="2:36" x14ac:dyDescent="0.25">
+      <c r="AJ77" s="24"/>
+      <c r="AK77" s="24"/>
+    </row>
+    <row r="78" spans="2:37" x14ac:dyDescent="0.25">
       <c r="B78" s="13">
         <v>30</v>
       </c>
@@ -1874,12 +1930,16 @@
       <c r="AH78">
         <v>93</v>
       </c>
-      <c r="AJ78">
+      <c r="AJ78" s="24">
         <f>AVERAGE(Y78:AH78)</f>
         <v>89.97</v>
       </c>
-    </row>
-    <row r="79" spans="2:36" x14ac:dyDescent="0.25">
+      <c r="AK78" s="24">
+        <f t="shared" si="1"/>
+        <v>65.5</v>
+      </c>
+    </row>
+    <row r="79" spans="2:37" x14ac:dyDescent="0.25">
       <c r="B79" s="16">
         <v>230</v>
       </c>
@@ -1931,12 +1991,16 @@
       <c r="AH79">
         <v>82.2</v>
       </c>
-      <c r="AJ79">
+      <c r="AJ79" s="24">
         <f>AVERAGE(Y79:AH79)</f>
         <v>80.97999999999999</v>
       </c>
-    </row>
-    <row r="80" spans="2:36" x14ac:dyDescent="0.25">
+      <c r="AK79" s="24">
+        <f t="shared" si="1"/>
+        <v>63.1</v>
+      </c>
+    </row>
+    <row r="80" spans="2:37" x14ac:dyDescent="0.25">
       <c r="B80" s="13">
         <v>20</v>
       </c>
@@ -1955,13 +2019,20 @@
       <c r="M80" s="1" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="81" spans="4:36" x14ac:dyDescent="0.25">
+      <c r="AJ80" s="24"/>
+      <c r="AK80" s="24">
+        <f t="shared" si="1"/>
+        <v>96.1</v>
+      </c>
+    </row>
+    <row r="81" spans="4:37" x14ac:dyDescent="0.25">
       <c r="D81" s="19" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="82" spans="4:36" x14ac:dyDescent="0.25">
+      <c r="AJ81" s="24"/>
+      <c r="AK81" s="24"/>
+    </row>
+    <row r="82" spans="4:37" x14ac:dyDescent="0.25">
       <c r="D82" s="13">
         <v>3.7</v>
       </c>
@@ -1974,13 +2045,17 @@
       <c r="M82" s="1" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="83" spans="4:36" x14ac:dyDescent="0.25">
+      <c r="AJ82" s="24"/>
+      <c r="AK82" s="24"/>
+    </row>
+    <row r="83" spans="4:37" x14ac:dyDescent="0.25">
       <c r="M83" s="1" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="84" spans="4:36" x14ac:dyDescent="0.25">
+      <c r="AJ83" s="24"/>
+      <c r="AK83" s="24"/>
+    </row>
+    <row r="84" spans="4:37" x14ac:dyDescent="0.25">
       <c r="D84" s="13">
         <v>3.1</v>
       </c>
@@ -2023,12 +2098,16 @@
       <c r="AH84">
         <v>76.400000000000006</v>
       </c>
-      <c r="AJ84">
-        <f t="shared" ref="AJ84" si="1">AVERAGE(Y84:AH84)</f>
+      <c r="AJ84" s="24">
+        <f t="shared" ref="AJ84" si="2">AVERAGE(Y84:AH84)</f>
         <v>77.400000000000006</v>
       </c>
-    </row>
-    <row r="85" spans="4:36" x14ac:dyDescent="0.25">
+      <c r="AK84" s="24">
+        <f t="shared" si="1"/>
+        <v>60.1</v>
+      </c>
+    </row>
+    <row r="85" spans="4:37" x14ac:dyDescent="0.25">
       <c r="D85" s="13">
         <v>3.8</v>
       </c>
@@ -2041,8 +2120,14 @@
       <c r="M85" s="1" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="87" spans="4:36" x14ac:dyDescent="0.25">
+      <c r="AJ85" s="24"/>
+      <c r="AK85" s="24"/>
+    </row>
+    <row r="86" spans="4:37" x14ac:dyDescent="0.25">
+      <c r="AJ86" s="24"/>
+      <c r="AK86" s="24"/>
+    </row>
+    <row r="87" spans="4:37" x14ac:dyDescent="0.25">
       <c r="D87" s="13">
         <v>6</v>
       </c>
@@ -2055,8 +2140,10 @@
       <c r="M87" s="1" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="88" spans="4:36" x14ac:dyDescent="0.25">
+      <c r="AJ87" s="24"/>
+      <c r="AK87" s="24"/>
+    </row>
+    <row r="88" spans="4:37" x14ac:dyDescent="0.25">
       <c r="D88" s="13">
         <v>7</v>
       </c>
@@ -2069,8 +2156,10 @@
       <c r="M88" s="1" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="89" spans="4:36" x14ac:dyDescent="0.25">
+      <c r="AJ88" s="24"/>
+      <c r="AK88" s="24"/>
+    </row>
+    <row r="89" spans="4:37" x14ac:dyDescent="0.25">
       <c r="D89" s="13">
         <v>2.5</v>
       </c>
@@ -2113,12 +2202,16 @@
       <c r="AH89">
         <v>86.9</v>
       </c>
-      <c r="AJ89">
-        <f t="shared" ref="AJ89" si="2">AVERAGE(Y89:AH89)</f>
+      <c r="AJ89" s="24">
+        <f t="shared" ref="AJ89" si="3">AVERAGE(Y89:AH89)</f>
         <v>83.402000000000001</v>
       </c>
-    </row>
-    <row r="90" spans="4:36" x14ac:dyDescent="0.25">
+      <c r="AK89" s="24">
+        <f t="shared" si="1"/>
+        <v>63.7</v>
+      </c>
+    </row>
+    <row r="90" spans="4:37" x14ac:dyDescent="0.25">
       <c r="D90" s="13">
         <v>6</v>
       </c>
@@ -2131,8 +2224,14 @@
       <c r="M90" s="1" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="92" spans="4:36" x14ac:dyDescent="0.25">
+      <c r="AJ90" s="24"/>
+      <c r="AK90" s="24"/>
+    </row>
+    <row r="91" spans="4:37" x14ac:dyDescent="0.25">
+      <c r="AJ91" s="24"/>
+      <c r="AK91" s="24"/>
+    </row>
+    <row r="92" spans="4:37" x14ac:dyDescent="0.25">
       <c r="D92" s="13">
         <v>6</v>
       </c>
@@ -2175,12 +2274,16 @@
       <c r="AH92">
         <v>85.8</v>
       </c>
-      <c r="AJ92">
-        <f t="shared" ref="AJ92:AJ94" si="3">AVERAGE(Y92:AH92)</f>
+      <c r="AJ92" s="24">
+        <f t="shared" ref="AJ92:AJ94" si="4">AVERAGE(Y92:AH92)</f>
         <v>76.16</v>
       </c>
-    </row>
-    <row r="93" spans="4:36" x14ac:dyDescent="0.25">
+      <c r="AK92" s="24">
+        <f t="shared" si="1"/>
+        <v>59.02</v>
+      </c>
+    </row>
+    <row r="93" spans="4:37" x14ac:dyDescent="0.25">
       <c r="D93" s="13">
         <v>5</v>
       </c>
@@ -2223,12 +2326,16 @@
       <c r="AH93">
         <v>89.6</v>
       </c>
-      <c r="AJ93">
-        <f t="shared" si="3"/>
+      <c r="AJ93" s="24">
+        <f t="shared" si="4"/>
         <v>73.950000000000017</v>
       </c>
-    </row>
-    <row r="94" spans="4:36" x14ac:dyDescent="0.25">
+      <c r="AK93" s="24">
+        <f t="shared" si="1"/>
+        <v>57.7</v>
+      </c>
+    </row>
+    <row r="94" spans="4:37" x14ac:dyDescent="0.25">
       <c r="D94" s="13" t="s">
         <v>93</v>
       </c>
@@ -2271,12 +2378,16 @@
       <c r="AH94">
         <v>81.900000000000006</v>
       </c>
-      <c r="AJ94">
-        <f t="shared" si="3"/>
+      <c r="AJ94" s="24">
+        <f t="shared" si="4"/>
         <v>78.978999999999999</v>
       </c>
-    </row>
-    <row r="95" spans="4:36" x14ac:dyDescent="0.25">
+      <c r="AK94" s="24">
+        <f t="shared" si="1"/>
+        <v>67.39</v>
+      </c>
+    </row>
+    <row r="95" spans="4:37" x14ac:dyDescent="0.25">
       <c r="D95" s="13">
         <v>6</v>
       </c>
@@ -2319,18 +2430,119 @@
       <c r="AH95">
         <v>85.9</v>
       </c>
-      <c r="AJ95">
+      <c r="AJ95" s="24">
         <f>AVERAGE(Y95:AH95)</f>
         <v>72.119999999999976</v>
       </c>
-    </row>
-    <row r="101" spans="13:13" x14ac:dyDescent="0.25">
+      <c r="AK95" s="24">
+        <f t="shared" si="1"/>
+        <v>56.5</v>
+      </c>
+    </row>
+    <row r="97" spans="5:13" x14ac:dyDescent="0.25">
+      <c r="E97" s="19" t="s">
+        <v>103</v>
+      </c>
+      <c r="M97" s="2" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="98" spans="5:13" x14ac:dyDescent="0.25">
+      <c r="E98" s="13">
+        <v>0.11</v>
+      </c>
+      <c r="G98" s="11">
+        <v>51.2</v>
+      </c>
+      <c r="H98" s="20">
+        <v>0.8</v>
+      </c>
+      <c r="M98" s="1" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="99" spans="5:13" x14ac:dyDescent="0.25">
+      <c r="E99" s="13">
+        <v>0.22</v>
+      </c>
+      <c r="G99" s="11">
+        <v>61.8</v>
+      </c>
+      <c r="H99" s="20">
+        <v>2.8</v>
+      </c>
+      <c r="M99" s="1" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="100" spans="5:13" x14ac:dyDescent="0.25">
+      <c r="E100" s="13">
+        <v>1.2</v>
+      </c>
+      <c r="G100" s="11">
+        <v>60.6</v>
+      </c>
+      <c r="H100" s="20">
+        <v>0.2</v>
+      </c>
+      <c r="M100" s="1" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="101" spans="5:13" x14ac:dyDescent="0.25">
       <c r="M101" s="2"/>
     </row>
-    <row r="111" spans="13:13" x14ac:dyDescent="0.25">
+    <row r="102" spans="5:13" x14ac:dyDescent="0.25">
+      <c r="M102" s="2" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="103" spans="5:13" x14ac:dyDescent="0.25">
+      <c r="E103" s="13">
+        <v>1.2</v>
+      </c>
+      <c r="G103" s="11">
+        <v>46.34</v>
+      </c>
+      <c r="H103" s="20">
+        <v>0</v>
+      </c>
+      <c r="M103" s="1" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="104" spans="5:13" x14ac:dyDescent="0.25">
+      <c r="E104" s="13">
+        <v>0.24</v>
+      </c>
+      <c r="G104" s="11">
+        <v>57.5</v>
+      </c>
+      <c r="H104" s="20">
+        <v>1.5</v>
+      </c>
+      <c r="M104" s="1" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="105" spans="5:13" x14ac:dyDescent="0.25">
+      <c r="E105" s="13">
+        <v>0.76</v>
+      </c>
+      <c r="G105" s="11">
+        <v>57.4</v>
+      </c>
+      <c r="H105" s="20">
+        <v>0.4</v>
+      </c>
+      <c r="M105" s="1" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="111" spans="5:13" x14ac:dyDescent="0.25">
       <c r="M111" s="2"/>
     </row>
-    <row r="112" spans="13:13" x14ac:dyDescent="0.25">
+    <row r="112" spans="5:13" x14ac:dyDescent="0.25">
       <c r="M112" s="2"/>
     </row>
     <row r="117" spans="4:13" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Fixed CRITICAL bug in linear function approximation in MABsolver! Improved modularity for linear function parameter selection
</commit_message>
<xml_diff>
--- a/matlab_analysis/Results.xlsx
+++ b/matlab_analysis/Results.xlsx
@@ -14,20 +14,14 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="106">
   <si>
     <t>conf</t>
   </si>
   <si>
-    <t>mean</t>
-  </si>
-  <si>
     <t>MEASURED SCORES</t>
   </si>
   <si>
-    <t>median</t>
-  </si>
-  <si>
     <t>best value</t>
   </si>
   <si>
@@ -329,6 +323,15 @@
   </si>
   <si>
     <t>avgMax</t>
+  </si>
+  <si>
+    <t>real</t>
+  </si>
+  <si>
+    <t>experiment_filenames{81}   = 'Reprint___2014_10_21_noCPD_UCBT_perStep50___2014_10_21_22_15_21';</t>
+  </si>
+  <si>
+    <t>experiment_filenames{82}   = 'Reprint___2014_10_21_noCPD_UCBT_perStep100___2014_10_21_22_15_25';</t>
   </si>
 </sst>
 </file>
@@ -339,7 +342,7 @@
     <numFmt numFmtId="164" formatCode="0.0"/>
     <numFmt numFmtId="165" formatCode="0.000"/>
   </numFmts>
-  <fonts count="15" x14ac:knownFonts="1">
+  <fonts count="17" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -459,6 +462,23 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF7030A0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="238"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF7030A0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="238"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -480,13 +500,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="2" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -531,6 +548,18 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="15" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="15" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="164" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -837,787 +866,785 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AK422"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="Z61" workbookViewId="0">
-      <selection activeCell="AM80" sqref="AM80"/>
+    <sheetView tabSelected="1" topLeftCell="X76" workbookViewId="0">
+      <selection activeCell="AH110" sqref="AH110"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="5" width="8" style="13" customWidth="1"/>
+    <col min="1" max="5" width="8" style="12" customWidth="1"/>
     <col min="6" max="6" width="8" customWidth="1"/>
-    <col min="7" max="7" width="11.7109375" style="11" customWidth="1"/>
-    <col min="8" max="8" width="5.5703125" style="20" customWidth="1"/>
-    <col min="9" max="9" width="2.7109375" style="5" customWidth="1"/>
-    <col min="10" max="11" width="5.5703125" style="5" customWidth="1"/>
-    <col min="12" max="12" width="1.5703125" style="5" customWidth="1"/>
+    <col min="7" max="7" width="11.7109375" style="10" customWidth="1"/>
+    <col min="8" max="8" width="5.5703125" style="19" customWidth="1"/>
+    <col min="9" max="9" width="2.7109375" style="4" customWidth="1"/>
+    <col min="10" max="10" width="5.5703125" style="30" customWidth="1"/>
+    <col min="11" max="11" width="5.5703125" style="19" customWidth="1"/>
+    <col min="12" max="12" width="1.5703125" style="4" customWidth="1"/>
     <col min="13" max="13" width="15.42578125" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="F1" s="2"/>
-      <c r="I1" s="4"/>
-      <c r="J1" s="3" t="s">
+      <c r="I1" s="3"/>
+      <c r="J1" s="27" t="s">
+        <v>1</v>
+      </c>
+      <c r="K1" s="20"/>
+      <c r="L1" s="3"/>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="E2" s="13"/>
+      <c r="F2" s="2"/>
+      <c r="G2" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="K1" s="4"/>
-      <c r="L1" s="4"/>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="E2" s="14"/>
-      <c r="F2" s="2"/>
-      <c r="G2" s="12" t="s">
-        <v>4</v>
-      </c>
-      <c r="H2" s="21" t="s">
+      <c r="H2" s="20" t="s">
         <v>0</v>
       </c>
-      <c r="I2" s="4"/>
-      <c r="J2" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="K2" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="L2" s="4"/>
+      <c r="I2" s="3"/>
+      <c r="J2" s="28" t="s">
+        <v>103</v>
+      </c>
+      <c r="K2" s="29" t="s">
+        <v>73</v>
+      </c>
+      <c r="L2" s="3"/>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="M4" s="2"/>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="M5" s="2" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="M7" s="1" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="M8" s="1" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="M9" s="1" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A10" s="15" t="s">
-        <v>22</v>
-      </c>
-      <c r="B10" s="15" t="s">
-        <v>21</v>
-      </c>
-      <c r="C10" s="15" t="s">
+      <c r="A10" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="D10" s="15" t="s">
+      <c r="B10" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="E10" s="15" t="s">
+      <c r="C10" s="14" t="s">
         <v>18</v>
       </c>
+      <c r="D10" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="E10" s="14" t="s">
+        <v>16</v>
+      </c>
       <c r="M10" s="1" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="M11" s="1" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="M13" s="2" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="M14" s="1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="M15" s="1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="M16" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="17" spans="5:13" x14ac:dyDescent="0.25">
+      <c r="M17" s="6" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="18" spans="5:13" x14ac:dyDescent="0.25">
+      <c r="E18" s="12">
+        <v>0.122</v>
+      </c>
+      <c r="G18" s="10">
+        <v>44.49</v>
+      </c>
+      <c r="M18" s="1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="17" spans="5:13" x14ac:dyDescent="0.25">
-      <c r="M17" s="7" t="s">
+    <row r="19" spans="5:13" x14ac:dyDescent="0.25">
+      <c r="E19" s="12">
+        <v>0.11</v>
+      </c>
+      <c r="G19" s="10">
+        <v>51.73</v>
+      </c>
+      <c r="M19" s="1" t="s">
         <v>13</v>
-      </c>
-    </row>
-    <row r="18" spans="5:13" x14ac:dyDescent="0.25">
-      <c r="E18" s="13">
-        <v>0.122</v>
-      </c>
-      <c r="G18" s="11">
-        <v>44.49</v>
-      </c>
-      <c r="M18" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="19" spans="5:13" x14ac:dyDescent="0.25">
-      <c r="E19" s="13">
-        <v>0.11</v>
-      </c>
-      <c r="G19" s="11">
-        <v>51.73</v>
-      </c>
-      <c r="M19" s="1" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="20" spans="5:13" x14ac:dyDescent="0.25">
       <c r="M20" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="22" spans="5:13" x14ac:dyDescent="0.25">
       <c r="M22" s="2" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="23" spans="5:13" x14ac:dyDescent="0.25">
-      <c r="E23" s="13">
+      <c r="E23" s="12">
         <v>0.12</v>
       </c>
-      <c r="G23" s="11">
+      <c r="G23" s="10">
         <v>73.400000000000006</v>
       </c>
       <c r="M23" s="1" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="24" spans="5:13" x14ac:dyDescent="0.25">
-      <c r="M24" s="7" t="s">
-        <v>17</v>
+      <c r="M24" s="6" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="25" spans="5:13" x14ac:dyDescent="0.25">
-      <c r="E25" s="13">
+      <c r="E25" s="12">
         <v>0.14000000000000001</v>
       </c>
-      <c r="G25" s="11">
+      <c r="G25" s="10">
         <v>68.900000000000006</v>
       </c>
       <c r="M25" s="1" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="26" spans="5:13" x14ac:dyDescent="0.25">
-      <c r="E26" s="13">
+      <c r="E26" s="12">
         <v>0.35</v>
       </c>
-      <c r="G26" s="11">
+      <c r="G26" s="10">
         <v>71.7</v>
       </c>
       <c r="M26" s="1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="27" spans="5:13" x14ac:dyDescent="0.25">
-      <c r="E27" s="13">
+      <c r="E27" s="12">
         <v>3.5999999999999997E-2</v>
       </c>
-      <c r="G27" s="11">
+      <c r="G27" s="10">
         <v>94.1</v>
       </c>
       <c r="M27" s="1" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="28" spans="5:13" x14ac:dyDescent="0.25">
       <c r="M28" s="1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="29" spans="5:13" x14ac:dyDescent="0.25">
-      <c r="E29" s="13">
+      <c r="E29" s="12">
         <v>0</v>
       </c>
-      <c r="G29" s="11">
+      <c r="G29" s="10">
         <v>99.83</v>
       </c>
       <c r="M29" s="1" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="30" spans="5:13" x14ac:dyDescent="0.25">
-      <c r="E30" s="13">
+      <c r="E30" s="12">
         <v>0</v>
       </c>
-      <c r="G30" s="11">
+      <c r="G30" s="10">
         <v>99.83</v>
       </c>
       <c r="M30" s="1" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="31" spans="5:13" x14ac:dyDescent="0.25">
       <c r="M31" s="2"/>
     </row>
     <row r="32" spans="5:13" x14ac:dyDescent="0.25">
-      <c r="E32" s="13">
+      <c r="E32" s="12">
         <v>0.06</v>
       </c>
-      <c r="G32" s="11">
+      <c r="G32" s="10">
         <v>35.6</v>
       </c>
-      <c r="M32" s="7" t="s">
+      <c r="M32" s="6" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="33" spans="5:36" x14ac:dyDescent="0.25">
+      <c r="M33" s="6" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="34" spans="5:36" x14ac:dyDescent="0.25">
+      <c r="E34" s="12">
+        <v>0.34</v>
+      </c>
+      <c r="G34" s="10">
+        <v>62.5</v>
+      </c>
+      <c r="M34" s="6" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="35" spans="5:36" x14ac:dyDescent="0.25">
+      <c r="E35" s="12">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="G35" s="10">
+        <v>64.099999999999994</v>
+      </c>
+      <c r="M35" s="6" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="36" spans="5:36" x14ac:dyDescent="0.25">
+      <c r="E36" s="12">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="G36" s="10">
+        <v>43.8</v>
+      </c>
+      <c r="M36" s="6" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="37" spans="5:36" x14ac:dyDescent="0.25">
+      <c r="M37" s="6" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="38" spans="5:36" x14ac:dyDescent="0.25">
+      <c r="E38" s="12">
+        <v>8.5000000000000006E-2</v>
+      </c>
+      <c r="G38" s="10">
+        <v>83.6</v>
+      </c>
+      <c r="M38" s="6" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="39" spans="5:36" x14ac:dyDescent="0.25">
+      <c r="E39" s="12">
+        <v>0.23</v>
+      </c>
+      <c r="G39" s="10">
+        <v>82.25</v>
+      </c>
+      <c r="M39" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="Y39" s="21"/>
+      <c r="AC39" s="21"/>
+      <c r="AD39" s="21"/>
+      <c r="AE39" s="21"/>
+      <c r="AF39" s="21"/>
+      <c r="AG39" s="21"/>
+      <c r="AH39" s="21"/>
+    </row>
+    <row r="40" spans="5:36" x14ac:dyDescent="0.25">
+      <c r="M40" s="6"/>
+      <c r="Y40" s="21"/>
+      <c r="Z40" s="21"/>
+      <c r="AA40" s="21"/>
+      <c r="AB40" s="21"/>
+      <c r="AC40" s="21"/>
+      <c r="AD40" s="21"/>
+      <c r="AE40" s="21"/>
+      <c r="AF40" s="21"/>
+      <c r="AG40" s="21"/>
+      <c r="AH40" s="21"/>
+      <c r="AJ40" s="21"/>
+    </row>
+    <row r="41" spans="5:36" x14ac:dyDescent="0.25">
+      <c r="E41" s="12">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="G41" s="10">
+        <v>48.3</v>
+      </c>
+      <c r="M41" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="Y41" s="25"/>
+      <c r="Z41" s="25"/>
+      <c r="AA41" s="25"/>
+      <c r="AB41" s="25"/>
+      <c r="AC41" s="25"/>
+      <c r="AD41" s="25"/>
+      <c r="AE41" s="25"/>
+      <c r="AF41" s="25"/>
+      <c r="AG41" s="25"/>
+      <c r="AH41" s="25"/>
+      <c r="AJ41" s="23"/>
+    </row>
+    <row r="42" spans="5:36" x14ac:dyDescent="0.25">
+      <c r="E42" s="12">
+        <v>1E-3</v>
+      </c>
+      <c r="G42" s="10">
+        <v>30.7</v>
+      </c>
+      <c r="J42" s="27"/>
+      <c r="M42" s="6" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="33" spans="5:36" x14ac:dyDescent="0.25">
-      <c r="M33" s="7" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="34" spans="5:36" x14ac:dyDescent="0.25">
-      <c r="E34" s="13">
-        <v>0.34</v>
-      </c>
-      <c r="G34" s="11">
-        <v>62.5</v>
-      </c>
-      <c r="M34" s="7" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="35" spans="5:36" x14ac:dyDescent="0.25">
-      <c r="E35" s="13">
-        <v>1.1000000000000001</v>
-      </c>
-      <c r="G35" s="11">
-        <v>64.099999999999994</v>
-      </c>
-      <c r="M35" s="7" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="36" spans="5:36" x14ac:dyDescent="0.25">
-      <c r="E36" s="13">
-        <v>5.0000000000000001E-3</v>
-      </c>
-      <c r="G36" s="11">
-        <v>43.8</v>
-      </c>
-      <c r="M36" s="7" t="s">
+    <row r="43" spans="5:36" x14ac:dyDescent="0.25">
+      <c r="E43" s="12">
+        <v>0.24</v>
+      </c>
+      <c r="F43" s="9"/>
+      <c r="G43" s="10">
+        <v>58.7</v>
+      </c>
+      <c r="H43" s="19">
+        <v>0.7</v>
+      </c>
+      <c r="M43" s="6" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="44" spans="5:36" x14ac:dyDescent="0.25">
+      <c r="E44" s="12">
+        <v>0.77</v>
+      </c>
+      <c r="G44" s="10">
+        <v>61.07</v>
+      </c>
+      <c r="H44" s="19">
+        <v>0.6</v>
+      </c>
+      <c r="M44" s="6" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="45" spans="5:36" x14ac:dyDescent="0.25">
+      <c r="E45" s="12">
+        <v>0.02</v>
+      </c>
+      <c r="G45" s="10">
+        <v>64.3</v>
+      </c>
+      <c r="M45" s="6" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="37" spans="5:36" x14ac:dyDescent="0.25">
-      <c r="M37" s="7" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="38" spans="5:36" x14ac:dyDescent="0.25">
-      <c r="E38" s="13">
-        <v>8.5000000000000006E-2</v>
-      </c>
-      <c r="G38" s="11">
-        <v>83.6</v>
-      </c>
-      <c r="M38" s="7" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="39" spans="5:36" x14ac:dyDescent="0.25">
-      <c r="E39" s="13">
-        <v>0.23</v>
-      </c>
-      <c r="G39" s="11">
-        <v>82.25</v>
-      </c>
-      <c r="M39" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="Y39" s="22"/>
-      <c r="AC39" s="22"/>
-      <c r="AD39" s="22"/>
-      <c r="AE39" s="22"/>
-      <c r="AF39" s="22"/>
-      <c r="AG39" s="22"/>
-      <c r="AH39" s="22"/>
-    </row>
-    <row r="40" spans="5:36" x14ac:dyDescent="0.25">
-      <c r="M40" s="7"/>
-      <c r="Y40" s="22"/>
-      <c r="Z40" s="22"/>
-      <c r="AA40" s="22"/>
-      <c r="AB40" s="22"/>
-      <c r="AC40" s="22"/>
-      <c r="AD40" s="22"/>
-      <c r="AE40" s="22"/>
-      <c r="AF40" s="22"/>
-      <c r="AG40" s="22"/>
-      <c r="AH40" s="22"/>
-      <c r="AJ40" s="22"/>
-    </row>
-    <row r="41" spans="5:36" x14ac:dyDescent="0.25">
-      <c r="E41" s="13">
-        <v>0.14000000000000001</v>
-      </c>
-      <c r="G41" s="11">
-        <v>48.3</v>
-      </c>
-      <c r="M41" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="Y41" s="26"/>
-      <c r="Z41" s="26"/>
-      <c r="AA41" s="26"/>
-      <c r="AB41" s="26"/>
-      <c r="AC41" s="26"/>
-      <c r="AD41" s="26"/>
-      <c r="AE41" s="26"/>
-      <c r="AF41" s="26"/>
-      <c r="AG41" s="26"/>
-      <c r="AH41" s="26"/>
-      <c r="AJ41" s="24"/>
-    </row>
-    <row r="42" spans="5:36" x14ac:dyDescent="0.25">
-      <c r="E42" s="13">
-        <v>1E-3</v>
-      </c>
-      <c r="G42" s="11">
-        <v>30.7</v>
-      </c>
-      <c r="J42" s="4"/>
-      <c r="M42" s="7" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="43" spans="5:36" x14ac:dyDescent="0.25">
-      <c r="E43" s="13">
-        <v>0.24</v>
-      </c>
-      <c r="F43" s="10"/>
-      <c r="G43" s="11">
-        <v>58.7</v>
-      </c>
-      <c r="H43" s="20">
-        <v>0.7</v>
-      </c>
-      <c r="M43" s="7" t="s">
+    <row r="46" spans="5:36" x14ac:dyDescent="0.25">
+      <c r="E46" s="12">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="G46" s="10">
+        <v>34.4</v>
+      </c>
+      <c r="M46" s="6" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="44" spans="5:36" x14ac:dyDescent="0.25">
-      <c r="E44" s="13">
-        <v>0.77</v>
-      </c>
-      <c r="G44" s="11">
-        <v>61.07</v>
-      </c>
-      <c r="H44" s="20">
-        <v>0.6</v>
-      </c>
-      <c r="M44" s="7" t="s">
+    <row r="47" spans="5:36" x14ac:dyDescent="0.25">
+      <c r="E47" s="12">
+        <v>5.8999999999999997E-2</v>
+      </c>
+      <c r="G47" s="10">
+        <v>76.790000000000006</v>
+      </c>
+      <c r="H47" s="19">
+        <v>0.2</v>
+      </c>
+      <c r="M47" s="6" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="45" spans="5:36" x14ac:dyDescent="0.25">
-      <c r="E45" s="13">
-        <v>0.02</v>
-      </c>
-      <c r="G45" s="11">
-        <v>64.3</v>
-      </c>
-      <c r="M45" s="7" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="46" spans="5:36" x14ac:dyDescent="0.25">
-      <c r="E46" s="13">
-        <v>3.0000000000000001E-3</v>
-      </c>
-      <c r="G46" s="11">
-        <v>34.4</v>
-      </c>
-      <c r="M46" s="7" t="s">
+    <row r="48" spans="5:36" x14ac:dyDescent="0.25">
+      <c r="E48" s="12">
+        <v>0.16600000000000001</v>
+      </c>
+      <c r="G48" s="10">
+        <v>76.64</v>
+      </c>
+      <c r="H48" s="19">
+        <v>0.1</v>
+      </c>
+      <c r="M48" s="6" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="47" spans="5:36" x14ac:dyDescent="0.25">
-      <c r="E47" s="13">
-        <v>5.8999999999999997E-2</v>
-      </c>
-      <c r="G47" s="11">
-        <v>76.790000000000006</v>
-      </c>
-      <c r="H47" s="20">
-        <v>0.2</v>
-      </c>
-      <c r="M47" s="7" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="48" spans="5:36" x14ac:dyDescent="0.25">
-      <c r="E48" s="13">
-        <v>0.16600000000000001</v>
-      </c>
-      <c r="G48" s="11">
-        <v>76.64</v>
-      </c>
-      <c r="H48" s="20">
-        <v>0.1</v>
-      </c>
-      <c r="M48" s="7" t="s">
-        <v>34</v>
-      </c>
-    </row>
     <row r="49" spans="4:13" x14ac:dyDescent="0.25">
-      <c r="M49" s="7"/>
+      <c r="M49" s="6"/>
     </row>
     <row r="50" spans="4:13" x14ac:dyDescent="0.25">
       <c r="M50" s="2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="51" spans="4:13" x14ac:dyDescent="0.25">
+      <c r="E51" s="12">
+        <v>3.82</v>
+      </c>
+      <c r="G51" s="10">
+        <v>60.2</v>
+      </c>
+      <c r="M51" s="6" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="52" spans="4:13" x14ac:dyDescent="0.25">
+      <c r="E52" s="12">
+        <v>3.34</v>
+      </c>
+      <c r="G52" s="10">
+        <v>60.9</v>
+      </c>
+      <c r="M52" s="6" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="51" spans="4:13" x14ac:dyDescent="0.25">
-      <c r="E51" s="13">
-        <v>3.82</v>
-      </c>
-      <c r="G51" s="11">
-        <v>60.2</v>
-      </c>
-      <c r="M51" s="7" t="s">
+    <row r="53" spans="4:13" x14ac:dyDescent="0.25">
+      <c r="E53" s="12">
+        <v>3.33</v>
+      </c>
+      <c r="G53" s="10">
+        <v>60.1</v>
+      </c>
+      <c r="M53" s="6" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="52" spans="4:13" x14ac:dyDescent="0.25">
-      <c r="E52" s="13">
-        <v>3.34</v>
-      </c>
-      <c r="G52" s="11">
-        <v>60.9</v>
-      </c>
-      <c r="M52" s="7" t="s">
+    <row r="54" spans="4:13" x14ac:dyDescent="0.25">
+      <c r="E54" s="12">
+        <v>0.51</v>
+      </c>
+      <c r="G54" s="10">
+        <v>66.7</v>
+      </c>
+      <c r="M54" s="6" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="53" spans="4:13" x14ac:dyDescent="0.25">
-      <c r="E53" s="13">
-        <v>3.33</v>
-      </c>
-      <c r="G53" s="11">
-        <v>60.1</v>
-      </c>
-      <c r="M53" s="7" t="s">
+    <row r="55" spans="4:13" x14ac:dyDescent="0.25">
+      <c r="D55" s="18" t="s">
+        <v>68</v>
+      </c>
+      <c r="E55" s="18" t="s">
+        <v>70</v>
+      </c>
+      <c r="J55" s="27"/>
+      <c r="M55" s="6"/>
+    </row>
+    <row r="56" spans="4:13" x14ac:dyDescent="0.25">
+      <c r="D56" s="12">
+        <v>6</v>
+      </c>
+      <c r="E56" s="12">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="F56" s="9"/>
+      <c r="G56" s="10">
+        <v>54.2</v>
+      </c>
+      <c r="H56" s="19">
+        <v>0.1</v>
+      </c>
+      <c r="I56" s="3"/>
+      <c r="J56" s="27"/>
+      <c r="M56" s="6" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="54" spans="4:13" x14ac:dyDescent="0.25">
-      <c r="E54" s="13">
-        <v>0.51</v>
-      </c>
-      <c r="G54" s="11">
-        <v>66.7</v>
-      </c>
-      <c r="M54" s="7" t="s">
+    <row r="57" spans="4:13" x14ac:dyDescent="0.25">
+      <c r="D57" s="12">
+        <v>6</v>
+      </c>
+      <c r="E57" s="12">
+        <v>0.75</v>
+      </c>
+      <c r="F57" s="3"/>
+      <c r="G57" s="10">
+        <v>55.7</v>
+      </c>
+      <c r="H57" s="19">
+        <v>1</v>
+      </c>
+      <c r="I57" s="3"/>
+      <c r="J57" s="27"/>
+      <c r="M57" s="6" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="55" spans="4:13" x14ac:dyDescent="0.25">
-      <c r="D55" s="19" t="s">
+    <row r="58" spans="4:13" x14ac:dyDescent="0.25">
+      <c r="D58" s="12">
+        <v>6.2</v>
+      </c>
+      <c r="E58" s="12">
+        <v>0.52</v>
+      </c>
+      <c r="F58" s="3"/>
+      <c r="G58" s="10">
+        <v>54.6</v>
+      </c>
+      <c r="H58" s="19">
+        <v>0.3</v>
+      </c>
+      <c r="M58" s="6" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="59" spans="4:13" x14ac:dyDescent="0.25">
+      <c r="D59" s="12">
+        <v>4.45</v>
+      </c>
+      <c r="E59" s="12">
+        <v>0.79</v>
+      </c>
+      <c r="G59" s="10">
+        <v>59.6</v>
+      </c>
+      <c r="H59" s="19">
+        <v>0.6</v>
+      </c>
+      <c r="M59" s="6" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="60" spans="4:13" x14ac:dyDescent="0.25">
+      <c r="M60" s="6"/>
+    </row>
+    <row r="61" spans="4:13" x14ac:dyDescent="0.25">
+      <c r="G61" s="10">
+        <v>56.1</v>
+      </c>
+      <c r="H61" s="19">
+        <v>0.5</v>
+      </c>
+      <c r="M61" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="62" spans="4:13" x14ac:dyDescent="0.25">
+      <c r="G62" s="10">
+        <v>56.2</v>
+      </c>
+      <c r="H62" s="19">
+        <v>2.6</v>
+      </c>
+      <c r="M62" s="1" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="63" spans="4:13" x14ac:dyDescent="0.25">
+      <c r="G63" s="10">
+        <v>55.1</v>
+      </c>
+      <c r="H63" s="19">
+        <v>0.2</v>
+      </c>
+      <c r="M63" s="1" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="64" spans="4:13" x14ac:dyDescent="0.25">
+      <c r="G64" s="10">
+        <v>55.6</v>
+      </c>
+      <c r="H64" s="19">
+        <v>0.2</v>
+      </c>
+      <c r="M64" s="1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="65" spans="2:37" x14ac:dyDescent="0.25">
+      <c r="D65" s="18" t="s">
+        <v>68</v>
+      </c>
+      <c r="E65" s="18" t="s">
         <v>70</v>
       </c>
-      <c r="E55" s="19" t="s">
-        <v>72</v>
-      </c>
-      <c r="J55" s="4"/>
-      <c r="M55" s="7"/>
-    </row>
-    <row r="56" spans="4:13" x14ac:dyDescent="0.25">
-      <c r="D56" s="13">
+    </row>
+    <row r="66" spans="2:37" x14ac:dyDescent="0.25">
+      <c r="D66" s="12">
+        <v>1.8</v>
+      </c>
+      <c r="E66" s="12">
+        <v>0.65</v>
+      </c>
+      <c r="F66" s="3"/>
+      <c r="G66" s="10">
+        <v>62.44</v>
+      </c>
+      <c r="H66" s="19">
+        <v>0.06</v>
+      </c>
+      <c r="M66" s="1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="67" spans="2:37" x14ac:dyDescent="0.25">
+      <c r="D67" s="12">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="E67" s="12">
+        <v>0.79</v>
+      </c>
+      <c r="F67" s="3"/>
+      <c r="G67" s="10">
+        <v>57.83</v>
+      </c>
+      <c r="H67" s="19">
+        <v>0.22</v>
+      </c>
+      <c r="M67" s="1" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="68" spans="2:37" x14ac:dyDescent="0.25">
+      <c r="D68" s="12">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="E68" s="12">
+        <v>0.83</v>
+      </c>
+      <c r="F68" s="3"/>
+      <c r="G68" s="10">
+        <v>57.44</v>
+      </c>
+      <c r="H68" s="19">
+        <v>0.7</v>
+      </c>
+      <c r="M68" s="1" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="69" spans="2:37" x14ac:dyDescent="0.25">
+      <c r="D69" s="12">
+        <v>0.5</v>
+      </c>
+      <c r="E69" s="12">
+        <v>1.1200000000000001</v>
+      </c>
+      <c r="G69" s="10">
+        <v>60.96</v>
+      </c>
+      <c r="H69" s="19">
+        <v>0</v>
+      </c>
+      <c r="M69" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="Y69" s="21" t="s">
+        <v>92</v>
+      </c>
+      <c r="AC69" s="21"/>
+      <c r="AD69" s="21"/>
+      <c r="AE69" s="21"/>
+      <c r="AF69" s="21"/>
+      <c r="AG69" s="21"/>
+      <c r="AH69" s="21"/>
+    </row>
+    <row r="70" spans="2:37" x14ac:dyDescent="0.25">
+      <c r="D70" s="18" t="s">
+        <v>69</v>
+      </c>
+      <c r="E70" s="18" t="s">
+        <v>68</v>
+      </c>
+      <c r="M70" s="6"/>
+      <c r="Y70" s="21">
+        <v>7</v>
+      </c>
+      <c r="Z70" s="21">
+        <v>8</v>
+      </c>
+      <c r="AA70" s="21">
+        <v>9</v>
+      </c>
+      <c r="AB70" s="21">
+        <v>10</v>
+      </c>
+      <c r="AC70" s="21">
+        <v>1</v>
+      </c>
+      <c r="AD70" s="21">
+        <v>2</v>
+      </c>
+      <c r="AE70" s="21">
+        <v>3</v>
+      </c>
+      <c r="AF70" s="21">
+        <v>4</v>
+      </c>
+      <c r="AG70" s="21">
+        <v>5</v>
+      </c>
+      <c r="AH70" s="21">
         <v>6</v>
       </c>
-      <c r="E56" s="13">
-        <v>0.55000000000000004</v>
-      </c>
-      <c r="F56" s="10"/>
-      <c r="G56" s="11">
-        <v>54.2</v>
-      </c>
-      <c r="H56" s="20">
-        <v>0.1</v>
-      </c>
-      <c r="I56" s="4"/>
-      <c r="J56" s="4"/>
-      <c r="M56" s="7" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="57" spans="4:13" x14ac:dyDescent="0.25">
-      <c r="D57" s="13">
-        <v>6</v>
-      </c>
-      <c r="E57" s="13">
-        <v>0.75</v>
-      </c>
-      <c r="F57" s="4"/>
-      <c r="G57" s="11">
-        <v>55.7</v>
-      </c>
-      <c r="H57" s="20">
-        <v>1</v>
-      </c>
-      <c r="I57" s="4"/>
-      <c r="J57" s="4"/>
-      <c r="M57" s="7" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="58" spans="4:13" x14ac:dyDescent="0.25">
-      <c r="D58" s="13">
-        <v>6.2</v>
-      </c>
-      <c r="E58" s="13">
-        <v>0.52</v>
-      </c>
-      <c r="F58" s="4"/>
-      <c r="G58" s="11">
-        <v>54.6</v>
-      </c>
-      <c r="H58" s="20">
-        <v>0.3</v>
-      </c>
-      <c r="M58" s="7" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="59" spans="4:13" x14ac:dyDescent="0.25">
-      <c r="D59" s="13">
-        <v>4.45</v>
-      </c>
-      <c r="E59" s="13">
-        <v>0.79</v>
-      </c>
-      <c r="G59" s="11">
-        <v>59.6</v>
-      </c>
-      <c r="H59" s="20">
-        <v>0.6</v>
-      </c>
-      <c r="M59" s="7" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="60" spans="4:13" x14ac:dyDescent="0.25">
-      <c r="M60" s="7"/>
-    </row>
-    <row r="61" spans="4:13" x14ac:dyDescent="0.25">
-      <c r="G61" s="11">
-        <v>56.1</v>
-      </c>
-      <c r="H61" s="20">
+      <c r="AJ70" s="26" t="s">
+        <v>102</v>
+      </c>
+      <c r="AK70" s="23" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="71" spans="2:37" x14ac:dyDescent="0.25">
+      <c r="D71" s="12">
+        <v>0.65500000000000003</v>
+      </c>
+      <c r="E71" s="12">
         <v>0.5</v>
       </c>
-      <c r="M61" s="1" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="62" spans="4:13" x14ac:dyDescent="0.25">
-      <c r="G62" s="11">
-        <v>56.2</v>
-      </c>
-      <c r="H62" s="20">
-        <v>2.6</v>
-      </c>
-      <c r="M62" s="1" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="63" spans="4:13" x14ac:dyDescent="0.25">
-      <c r="G63" s="11">
-        <v>55.1</v>
-      </c>
-      <c r="H63" s="20">
-        <v>0.2</v>
-      </c>
-      <c r="M63" s="1" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="64" spans="4:13" x14ac:dyDescent="0.25">
-      <c r="G64" s="11">
-        <v>55.6</v>
-      </c>
-      <c r="H64" s="20">
-        <v>0.2</v>
-      </c>
-      <c r="M64" s="1" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="65" spans="2:37" x14ac:dyDescent="0.25">
-      <c r="D65" s="19" t="s">
-        <v>70</v>
-      </c>
-      <c r="E65" s="19" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="66" spans="2:37" x14ac:dyDescent="0.25">
-      <c r="D66" s="13">
-        <v>1.8</v>
-      </c>
-      <c r="E66" s="13">
-        <v>0.65</v>
-      </c>
-      <c r="F66" s="4"/>
-      <c r="G66" s="11">
-        <v>62.44</v>
-      </c>
-      <c r="H66" s="20">
-        <v>0.06</v>
-      </c>
-      <c r="M66" s="1" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="67" spans="2:37" x14ac:dyDescent="0.25">
-      <c r="D67" s="13">
-        <v>2.2999999999999998</v>
-      </c>
-      <c r="E67" s="13">
-        <v>0.79</v>
-      </c>
-      <c r="F67" s="4"/>
-      <c r="G67" s="11">
-        <v>57.83</v>
-      </c>
-      <c r="H67" s="20">
-        <v>0.22</v>
-      </c>
-      <c r="M67" s="1" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="68" spans="2:37" x14ac:dyDescent="0.25">
-      <c r="D68" s="13">
-        <v>2.2000000000000002</v>
-      </c>
-      <c r="E68" s="13">
-        <v>0.83</v>
-      </c>
-      <c r="F68" s="4"/>
-      <c r="G68" s="11">
-        <v>57.44</v>
-      </c>
-      <c r="H68" s="20">
-        <v>0.7</v>
-      </c>
-      <c r="M68" s="1" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="69" spans="2:37" x14ac:dyDescent="0.25">
-      <c r="D69" s="13">
-        <v>0.5</v>
-      </c>
-      <c r="E69" s="13">
-        <v>1.1200000000000001</v>
-      </c>
-      <c r="G69" s="11">
-        <v>60.96</v>
-      </c>
-      <c r="H69" s="20">
+      <c r="G71" s="10">
+        <v>83.4</v>
+      </c>
+      <c r="H71" s="19">
         <v>0</v>
       </c>
-      <c r="M69" s="7" t="s">
-        <v>65</v>
-      </c>
-      <c r="Y69" s="22" t="s">
-        <v>94</v>
-      </c>
-      <c r="AC69" s="22"/>
-      <c r="AD69" s="22"/>
-      <c r="AE69" s="22"/>
-      <c r="AF69" s="22"/>
-      <c r="AG69" s="22"/>
-      <c r="AH69" s="22"/>
-    </row>
-    <row r="70" spans="2:37" x14ac:dyDescent="0.25">
-      <c r="D70" s="19" t="s">
-        <v>71</v>
-      </c>
-      <c r="E70" s="19" t="s">
-        <v>70</v>
-      </c>
-      <c r="J70" s="5" t="s">
-        <v>75</v>
-      </c>
-      <c r="M70" s="7"/>
-      <c r="Y70" s="22">
-        <v>7</v>
-      </c>
-      <c r="Z70" s="22">
-        <v>8</v>
-      </c>
-      <c r="AA70" s="22">
-        <v>9</v>
-      </c>
-      <c r="AB70" s="22">
-        <v>10</v>
-      </c>
-      <c r="AC70" s="22">
-        <v>1</v>
-      </c>
-      <c r="AD70" s="22">
-        <v>2</v>
-      </c>
-      <c r="AE70" s="22">
-        <v>3</v>
-      </c>
-      <c r="AF70" s="22">
-        <v>4</v>
-      </c>
-      <c r="AG70" s="22">
-        <v>5</v>
-      </c>
-      <c r="AH70" s="22">
-        <v>6</v>
-      </c>
-      <c r="AJ70" s="27" t="s">
-        <v>104</v>
-      </c>
-      <c r="AK70" s="24" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="71" spans="2:37" x14ac:dyDescent="0.25">
-      <c r="D71" s="13">
-        <v>0.65500000000000003</v>
-      </c>
-      <c r="E71" s="13">
-        <v>0.5</v>
-      </c>
-      <c r="G71" s="11">
-        <v>83.4</v>
-      </c>
-      <c r="H71" s="20">
-        <v>0</v>
-      </c>
-      <c r="J71" s="11">
+      <c r="K71" s="19">
         <f>AJ71</f>
         <v>83.911000000000001</v>
       </c>
       <c r="M71" s="1" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="Y71">
         <v>93.3</v>
       </c>
-      <c r="Z71" s="25">
+      <c r="Z71" s="24">
         <v>97.9</v>
       </c>
       <c r="AA71">
@@ -1644,36 +1671,36 @@
       <c r="AH71">
         <v>99.4</v>
       </c>
-      <c r="AJ71" s="24">
+      <c r="AJ71" s="23">
         <f>AVERAGE(Y71:AH71)</f>
         <v>83.911000000000001</v>
       </c>
-      <c r="AK71" s="24">
+      <c r="AK71" s="23">
         <f>G71</f>
         <v>83.4</v>
       </c>
     </row>
     <row r="72" spans="2:37" x14ac:dyDescent="0.25">
-      <c r="D72" s="13">
+      <c r="D72" s="12">
         <v>0.99</v>
       </c>
-      <c r="E72" s="13">
+      <c r="E72" s="12">
         <v>1.2</v>
       </c>
-      <c r="G72" s="11">
+      <c r="G72" s="10">
         <v>84.78</v>
       </c>
-      <c r="H72" s="20">
+      <c r="H72" s="19">
         <v>0</v>
       </c>
-      <c r="J72" s="11">
+      <c r="K72" s="19">
         <f>AJ72</f>
         <v>85.361000000000004</v>
       </c>
       <c r="M72" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="Y72" s="25">
+        <v>65</v>
+      </c>
+      <c r="Y72" s="24">
         <v>94.9</v>
       </c>
       <c r="Z72">
@@ -1682,7 +1709,7 @@
       <c r="AA72">
         <v>100</v>
       </c>
-      <c r="AB72" s="25">
+      <c r="AB72" s="24">
         <v>95.7</v>
       </c>
       <c r="AC72">
@@ -1709,34 +1736,34 @@
         <f t="shared" si="0"/>
         <v>99.4</v>
       </c>
-      <c r="AJ72" s="24">
+      <c r="AJ72" s="23">
         <f>AVERAGE(Y72:AH72)</f>
         <v>85.361000000000004</v>
       </c>
-      <c r="AK72" s="24">
+      <c r="AK72" s="23">
         <f t="shared" ref="AK72:AK95" si="1">G72</f>
         <v>84.78</v>
       </c>
     </row>
     <row r="73" spans="2:37" x14ac:dyDescent="0.25">
-      <c r="D73" s="13">
+      <c r="D73" s="12">
         <v>0.5</v>
       </c>
-      <c r="E73" s="13">
+      <c r="E73" s="12">
         <v>0.5</v>
       </c>
-      <c r="G73" s="11">
+      <c r="G73" s="10">
         <v>82.67</v>
       </c>
-      <c r="H73" s="20">
+      <c r="H73" s="19">
         <v>0</v>
       </c>
-      <c r="J73" s="11">
+      <c r="K73" s="19">
         <f>AJ73</f>
         <v>83.061000000000007</v>
       </c>
       <c r="M73" s="1" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="Y73">
         <v>86.5</v>
@@ -1774,34 +1801,34 @@
         <f t="shared" si="0"/>
         <v>99.4</v>
       </c>
-      <c r="AJ73" s="24">
+      <c r="AJ73" s="23">
         <f>AVERAGE(Y73:AH73)</f>
         <v>83.061000000000007</v>
       </c>
-      <c r="AK73" s="24">
+      <c r="AK73" s="23">
         <f t="shared" si="1"/>
         <v>82.67</v>
       </c>
     </row>
     <row r="74" spans="2:37" x14ac:dyDescent="0.25">
-      <c r="D74" s="13">
+      <c r="D74" s="12">
         <v>1</v>
       </c>
-      <c r="E74" s="13">
+      <c r="E74" s="12">
         <v>1.54</v>
       </c>
-      <c r="G74" s="11">
+      <c r="G74" s="10">
         <v>84.97</v>
       </c>
-      <c r="H74" s="20">
+      <c r="H74" s="19">
         <v>0</v>
       </c>
-      <c r="J74" s="11">
+      <c r="K74" s="19">
         <f>AJ74</f>
         <v>85.010999999999996</v>
       </c>
       <c r="M74" s="1" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="Y74">
         <v>94.5</v>
@@ -1839,66 +1866,70 @@
         <f t="shared" si="0"/>
         <v>99.4</v>
       </c>
-      <c r="AJ74" s="24">
+      <c r="AJ74" s="23">
         <f>AVERAGE(Y74:AH74)</f>
         <v>85.010999999999996</v>
       </c>
-      <c r="AK74" s="24">
+      <c r="AK74" s="23">
         <f t="shared" si="1"/>
         <v>84.97</v>
       </c>
     </row>
     <row r="75" spans="2:37" x14ac:dyDescent="0.25">
-      <c r="E75" s="23" t="s">
-        <v>74</v>
-      </c>
-      <c r="AJ75" s="24"/>
-      <c r="AK75" s="24"/>
+      <c r="E75" s="22" t="s">
+        <v>72</v>
+      </c>
+      <c r="AJ75" s="23"/>
+      <c r="AK75" s="23"/>
     </row>
     <row r="76" spans="2:37" x14ac:dyDescent="0.25">
       <c r="M76" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="AJ76" s="23"/>
+      <c r="AK76" s="23"/>
+    </row>
+    <row r="77" spans="2:37" x14ac:dyDescent="0.25">
+      <c r="B77" s="18" t="s">
         <v>76</v>
       </c>
-      <c r="AJ76" s="24"/>
-      <c r="AK76" s="24"/>
-    </row>
-    <row r="77" spans="2:37" x14ac:dyDescent="0.25">
-      <c r="B77" s="19" t="s">
-        <v>78</v>
-      </c>
-      <c r="C77" s="19" t="s">
-        <v>71</v>
-      </c>
-      <c r="D77" s="19" t="s">
+      <c r="C77" s="18" t="s">
+        <v>69</v>
+      </c>
+      <c r="D77" s="18" t="s">
+        <v>68</v>
+      </c>
+      <c r="E77" s="18" t="s">
         <v>70</v>
       </c>
-      <c r="E77" s="19" t="s">
-        <v>72</v>
-      </c>
-      <c r="AJ77" s="24"/>
-      <c r="AK77" s="24"/>
+      <c r="AJ77" s="23"/>
+      <c r="AK77" s="23"/>
     </row>
     <row r="78" spans="2:37" x14ac:dyDescent="0.25">
-      <c r="B78" s="13">
+      <c r="B78" s="12">
         <v>30</v>
       </c>
-      <c r="C78" s="13">
+      <c r="C78" s="12">
         <v>0.9</v>
       </c>
-      <c r="D78" s="13">
+      <c r="D78" s="12">
         <v>1.6</v>
       </c>
-      <c r="E78" s="13">
+      <c r="E78" s="12">
         <v>0.8</v>
       </c>
-      <c r="G78" s="11">
+      <c r="G78" s="10">
         <v>65.5</v>
       </c>
-      <c r="H78" s="20">
+      <c r="H78" s="19">
         <v>0.6</v>
       </c>
+      <c r="J78" s="30">
+        <f>G78-H78</f>
+        <v>64.900000000000006</v>
+      </c>
       <c r="M78" s="1" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="Y78">
         <v>79.7</v>
@@ -1930,36 +1961,40 @@
       <c r="AH78">
         <v>93</v>
       </c>
-      <c r="AJ78" s="24">
+      <c r="AJ78" s="23">
         <f>AVERAGE(Y78:AH78)</f>
         <v>89.97</v>
       </c>
-      <c r="AK78" s="24">
+      <c r="AK78" s="23">
         <f t="shared" si="1"/>
         <v>65.5</v>
       </c>
     </row>
     <row r="79" spans="2:37" x14ac:dyDescent="0.25">
-      <c r="B79" s="16">
+      <c r="B79" s="15">
         <v>230</v>
       </c>
-      <c r="C79" s="13">
+      <c r="C79" s="12">
         <v>1</v>
       </c>
-      <c r="D79" s="16">
+      <c r="D79" s="15">
         <v>0.95</v>
       </c>
-      <c r="E79" s="13">
+      <c r="E79" s="12">
         <v>0.77</v>
       </c>
-      <c r="G79" s="11">
+      <c r="G79" s="10">
         <v>63.1</v>
       </c>
-      <c r="H79" s="20">
+      <c r="H79" s="19">
         <v>1.2</v>
       </c>
+      <c r="J79" s="30">
+        <f t="shared" ref="J79:J107" si="2">G79-H79</f>
+        <v>61.9</v>
+      </c>
       <c r="M79" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="Y79">
         <v>77.7</v>
@@ -1991,82 +2026,94 @@
       <c r="AH79">
         <v>82.2</v>
       </c>
-      <c r="AJ79" s="24">
+      <c r="AJ79" s="23">
         <f>AVERAGE(Y79:AH79)</f>
         <v>80.97999999999999</v>
       </c>
-      <c r="AK79" s="24">
+      <c r="AK79" s="23">
         <f t="shared" si="1"/>
         <v>63.1</v>
       </c>
     </row>
     <row r="80" spans="2:37" x14ac:dyDescent="0.25">
-      <c r="B80" s="13">
+      <c r="B80" s="12">
         <v>20</v>
       </c>
-      <c r="C80" s="13">
+      <c r="C80" s="12">
         <v>1</v>
       </c>
-      <c r="D80" s="13">
+      <c r="D80" s="12">
         <v>1</v>
       </c>
-      <c r="G80" s="11">
+      <c r="G80" s="10">
         <v>96.1</v>
       </c>
-      <c r="H80" s="20">
+      <c r="H80" s="19">
         <v>0.04</v>
       </c>
+      <c r="J80" s="30">
+        <f t="shared" si="2"/>
+        <v>96.059999999999988</v>
+      </c>
       <c r="M80" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="AJ80" s="24"/>
-      <c r="AK80" s="24">
+        <v>78</v>
+      </c>
+      <c r="AJ80" s="23"/>
+      <c r="AK80" s="23">
         <f t="shared" si="1"/>
         <v>96.1</v>
       </c>
     </row>
     <row r="81" spans="4:37" x14ac:dyDescent="0.25">
-      <c r="D81" s="19" t="s">
-        <v>70</v>
-      </c>
-      <c r="AJ81" s="24"/>
-      <c r="AK81" s="24"/>
+      <c r="D81" s="18" t="s">
+        <v>68</v>
+      </c>
+      <c r="AJ81" s="23"/>
+      <c r="AK81" s="23"/>
     </row>
     <row r="82" spans="4:37" x14ac:dyDescent="0.25">
-      <c r="D82" s="13">
+      <c r="D82" s="12">
         <v>3.7</v>
       </c>
-      <c r="G82" s="11">
+      <c r="G82" s="10">
         <v>61.4</v>
       </c>
-      <c r="H82" s="20">
+      <c r="H82" s="19">
         <v>1.4</v>
       </c>
+      <c r="J82" s="30">
+        <f t="shared" si="2"/>
+        <v>60</v>
+      </c>
       <c r="M82" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="AJ82" s="24"/>
-      <c r="AK82" s="24"/>
+        <v>79</v>
+      </c>
+      <c r="AJ82" s="23"/>
+      <c r="AK82" s="23"/>
     </row>
     <row r="83" spans="4:37" x14ac:dyDescent="0.25">
       <c r="M83" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="AJ83" s="24"/>
-      <c r="AK83" s="24"/>
+        <v>80</v>
+      </c>
+      <c r="AJ83" s="23"/>
+      <c r="AK83" s="23"/>
     </row>
     <row r="84" spans="4:37" x14ac:dyDescent="0.25">
-      <c r="D84" s="13">
+      <c r="D84" s="12">
         <v>3.1</v>
       </c>
-      <c r="G84" s="11">
+      <c r="G84" s="10">
         <v>60.1</v>
       </c>
-      <c r="H84" s="20">
+      <c r="H84" s="19">
         <v>1.6</v>
       </c>
-      <c r="M84" s="7" t="s">
-        <v>83</v>
+      <c r="J84" s="30">
+        <f t="shared" si="2"/>
+        <v>58.5</v>
+      </c>
+      <c r="M84" s="6" t="s">
+        <v>81</v>
       </c>
       <c r="Y84">
         <v>60.7</v>
@@ -2098,79 +2145,95 @@
       <c r="AH84">
         <v>76.400000000000006</v>
       </c>
-      <c r="AJ84" s="24">
-        <f t="shared" ref="AJ84" si="2">AVERAGE(Y84:AH84)</f>
+      <c r="AJ84" s="23">
+        <f t="shared" ref="AJ84" si="3">AVERAGE(Y84:AH84)</f>
         <v>77.400000000000006</v>
       </c>
-      <c r="AK84" s="24">
+      <c r="AK84" s="23">
         <f t="shared" si="1"/>
         <v>60.1</v>
       </c>
     </row>
     <row r="85" spans="4:37" x14ac:dyDescent="0.25">
-      <c r="D85" s="13">
+      <c r="D85" s="12">
         <v>3.8</v>
       </c>
-      <c r="G85" s="11">
+      <c r="G85" s="10">
         <v>58</v>
       </c>
-      <c r="H85" s="20">
+      <c r="H85" s="19">
         <v>0.6</v>
       </c>
+      <c r="J85" s="30">
+        <f t="shared" si="2"/>
+        <v>57.4</v>
+      </c>
       <c r="M85" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="AJ85" s="23"/>
+      <c r="AK85" s="23"/>
+    </row>
+    <row r="86" spans="4:37" x14ac:dyDescent="0.25">
+      <c r="AJ86" s="23"/>
+      <c r="AK86" s="23"/>
+    </row>
+    <row r="87" spans="4:37" x14ac:dyDescent="0.25">
+      <c r="D87" s="12">
+        <v>6</v>
+      </c>
+      <c r="G87" s="10">
+        <v>59.3</v>
+      </c>
+      <c r="H87" s="19">
+        <v>0.9</v>
+      </c>
+      <c r="J87" s="30">
+        <f t="shared" si="2"/>
+        <v>58.4</v>
+      </c>
+      <c r="M87" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="AJ87" s="23"/>
+      <c r="AK87" s="23"/>
+    </row>
+    <row r="88" spans="4:37" x14ac:dyDescent="0.25">
+      <c r="D88" s="12">
+        <v>7</v>
+      </c>
+      <c r="G88" s="10">
+        <v>57.8</v>
+      </c>
+      <c r="H88" s="19">
+        <v>1</v>
+      </c>
+      <c r="J88" s="30">
+        <f t="shared" si="2"/>
+        <v>56.8</v>
+      </c>
+      <c r="M88" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="AJ85" s="24"/>
-      <c r="AK85" s="24"/>
-    </row>
-    <row r="86" spans="4:37" x14ac:dyDescent="0.25">
-      <c r="AJ86" s="24"/>
-      <c r="AK86" s="24"/>
-    </row>
-    <row r="87" spans="4:37" x14ac:dyDescent="0.25">
-      <c r="D87" s="13">
-        <v>6</v>
-      </c>
-      <c r="G87" s="11">
-        <v>59.3</v>
-      </c>
-      <c r="H87" s="20">
-        <v>0.9</v>
-      </c>
-      <c r="M87" s="1" t="s">
+      <c r="AJ88" s="23"/>
+      <c r="AK88" s="23"/>
+    </row>
+    <row r="89" spans="4:37" x14ac:dyDescent="0.25">
+      <c r="D89" s="12">
+        <v>2.5</v>
+      </c>
+      <c r="G89" s="10">
+        <v>63.7</v>
+      </c>
+      <c r="H89" s="19">
+        <v>0.7</v>
+      </c>
+      <c r="J89" s="30">
+        <f t="shared" si="2"/>
+        <v>63</v>
+      </c>
+      <c r="M89" s="1" t="s">
         <v>85</v>
-      </c>
-      <c r="AJ87" s="24"/>
-      <c r="AK87" s="24"/>
-    </row>
-    <row r="88" spans="4:37" x14ac:dyDescent="0.25">
-      <c r="D88" s="13">
-        <v>7</v>
-      </c>
-      <c r="G88" s="11">
-        <v>57.8</v>
-      </c>
-      <c r="H88" s="20">
-        <v>1</v>
-      </c>
-      <c r="M88" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="AJ88" s="24"/>
-      <c r="AK88" s="24"/>
-    </row>
-    <row r="89" spans="4:37" x14ac:dyDescent="0.25">
-      <c r="D89" s="13">
-        <v>2.5</v>
-      </c>
-      <c r="G89" s="11">
-        <v>63.7</v>
-      </c>
-      <c r="H89" s="20">
-        <v>0.7</v>
-      </c>
-      <c r="M89" s="1" t="s">
-        <v>87</v>
       </c>
       <c r="Y89">
         <v>73.400000000000006</v>
@@ -2202,47 +2265,55 @@
       <c r="AH89">
         <v>86.9</v>
       </c>
-      <c r="AJ89" s="24">
-        <f t="shared" ref="AJ89" si="3">AVERAGE(Y89:AH89)</f>
+      <c r="AJ89" s="23">
+        <f t="shared" ref="AJ89" si="4">AVERAGE(Y89:AH89)</f>
         <v>83.402000000000001</v>
       </c>
-      <c r="AK89" s="24">
+      <c r="AK89" s="23">
         <f t="shared" si="1"/>
         <v>63.7</v>
       </c>
     </row>
     <row r="90" spans="4:37" x14ac:dyDescent="0.25">
-      <c r="D90" s="13">
+      <c r="D90" s="12">
         <v>6</v>
       </c>
-      <c r="G90" s="11">
+      <c r="G90" s="10">
         <v>58.47</v>
       </c>
-      <c r="H90" s="20">
+      <c r="H90" s="19">
         <v>1.1000000000000001</v>
       </c>
+      <c r="J90" s="30">
+        <f t="shared" si="2"/>
+        <v>57.37</v>
+      </c>
       <c r="M90" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="AJ90" s="24"/>
-      <c r="AK90" s="24"/>
+        <v>86</v>
+      </c>
+      <c r="AJ90" s="23"/>
+      <c r="AK90" s="23"/>
     </row>
     <row r="91" spans="4:37" x14ac:dyDescent="0.25">
-      <c r="AJ91" s="24"/>
-      <c r="AK91" s="24"/>
+      <c r="AJ91" s="23"/>
+      <c r="AK91" s="23"/>
     </row>
     <row r="92" spans="4:37" x14ac:dyDescent="0.25">
-      <c r="D92" s="13">
+      <c r="D92" s="12">
         <v>6</v>
       </c>
-      <c r="G92" s="11">
+      <c r="G92" s="10">
         <v>59.02</v>
       </c>
-      <c r="H92" s="20">
+      <c r="H92" s="19">
         <v>1.3</v>
       </c>
-      <c r="M92" s="7" t="s">
-        <v>89</v>
+      <c r="J92" s="30">
+        <f t="shared" si="2"/>
+        <v>57.720000000000006</v>
+      </c>
+      <c r="M92" s="6" t="s">
+        <v>87</v>
       </c>
       <c r="Y92">
         <v>69.5</v>
@@ -2274,27 +2345,31 @@
       <c r="AH92">
         <v>85.8</v>
       </c>
-      <c r="AJ92" s="24">
-        <f t="shared" ref="AJ92:AJ94" si="4">AVERAGE(Y92:AH92)</f>
+      <c r="AJ92" s="23">
+        <f t="shared" ref="AJ92:AJ94" si="5">AVERAGE(Y92:AH92)</f>
         <v>76.16</v>
       </c>
-      <c r="AK92" s="24">
+      <c r="AK92" s="23">
         <f t="shared" si="1"/>
         <v>59.02</v>
       </c>
     </row>
     <row r="93" spans="4:37" x14ac:dyDescent="0.25">
-      <c r="D93" s="13">
+      <c r="D93" s="12">
         <v>5</v>
       </c>
-      <c r="G93" s="11">
+      <c r="G93" s="10">
         <v>57.7</v>
       </c>
-      <c r="H93" s="20">
+      <c r="H93" s="19">
         <v>1.1000000000000001</v>
       </c>
+      <c r="J93" s="30">
+        <f t="shared" si="2"/>
+        <v>56.6</v>
+      </c>
       <c r="M93" s="1" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="Y93">
         <v>67.5</v>
@@ -2326,27 +2401,31 @@
       <c r="AH93">
         <v>89.6</v>
       </c>
-      <c r="AJ93" s="24">
-        <f t="shared" si="4"/>
+      <c r="AJ93" s="23">
+        <f t="shared" si="5"/>
         <v>73.950000000000017</v>
       </c>
-      <c r="AK93" s="24">
+      <c r="AK93" s="23">
         <f t="shared" si="1"/>
         <v>57.7</v>
       </c>
     </row>
     <row r="94" spans="4:37" x14ac:dyDescent="0.25">
-      <c r="D94" s="13" t="s">
-        <v>93</v>
-      </c>
-      <c r="G94" s="11">
+      <c r="D94" s="12" t="s">
+        <v>91</v>
+      </c>
+      <c r="G94" s="10">
         <v>67.39</v>
       </c>
-      <c r="H94" s="20">
+      <c r="H94" s="19">
         <v>1.1000000000000001</v>
       </c>
+      <c r="J94" s="30">
+        <f t="shared" si="2"/>
+        <v>66.290000000000006</v>
+      </c>
       <c r="M94" s="1" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="Y94">
         <v>68.599999999999994</v>
@@ -2378,27 +2457,31 @@
       <c r="AH94">
         <v>81.900000000000006</v>
       </c>
-      <c r="AJ94" s="24">
-        <f t="shared" si="4"/>
+      <c r="AJ94" s="23">
+        <f t="shared" si="5"/>
         <v>78.978999999999999</v>
       </c>
-      <c r="AK94" s="24">
+      <c r="AK94" s="23">
         <f t="shared" si="1"/>
         <v>67.39</v>
       </c>
     </row>
     <row r="95" spans="4:37" x14ac:dyDescent="0.25">
-      <c r="D95" s="13">
+      <c r="D95" s="12">
         <v>6</v>
       </c>
-      <c r="G95" s="11">
+      <c r="G95" s="10">
         <v>56.5</v>
       </c>
-      <c r="H95" s="20">
+      <c r="H95" s="19">
         <v>1.5</v>
       </c>
+      <c r="J95" s="30">
+        <f t="shared" si="2"/>
+        <v>55</v>
+      </c>
       <c r="M95" s="1" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="Y95">
         <v>66.8</v>
@@ -2430,119 +2513,255 @@
       <c r="AH95">
         <v>85.9</v>
       </c>
-      <c r="AJ95" s="24">
+      <c r="AJ95" s="23">
         <f>AVERAGE(Y95:AH95)</f>
         <v>72.119999999999976</v>
       </c>
-      <c r="AK95" s="24">
+      <c r="AK95" s="23">
         <f t="shared" si="1"/>
         <v>56.5</v>
       </c>
     </row>
-    <row r="97" spans="5:13" x14ac:dyDescent="0.25">
-      <c r="E97" s="19" t="s">
+    <row r="97" spans="5:37" x14ac:dyDescent="0.25">
+      <c r="E97" s="18" t="s">
+        <v>101</v>
+      </c>
+      <c r="M97" s="2" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="98" spans="5:37" x14ac:dyDescent="0.25">
+      <c r="E98" s="12">
+        <v>0.11</v>
+      </c>
+      <c r="G98" s="10">
+        <v>51.2</v>
+      </c>
+      <c r="H98" s="19">
+        <v>0.8</v>
+      </c>
+      <c r="J98" s="30">
+        <f t="shared" si="2"/>
+        <v>50.400000000000006</v>
+      </c>
+      <c r="M98" s="1" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="99" spans="5:37" x14ac:dyDescent="0.25">
+      <c r="E99" s="12">
+        <v>0.22</v>
+      </c>
+      <c r="G99" s="10">
+        <v>61.8</v>
+      </c>
+      <c r="H99" s="19">
+        <v>2.8</v>
+      </c>
+      <c r="J99" s="30">
+        <f t="shared" si="2"/>
+        <v>59</v>
+      </c>
+      <c r="M99" s="1" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="100" spans="5:37" x14ac:dyDescent="0.25">
+      <c r="E100" s="12">
+        <v>1.2</v>
+      </c>
+      <c r="G100" s="10">
+        <v>60.6</v>
+      </c>
+      <c r="H100" s="19">
+        <v>0.2</v>
+      </c>
+      <c r="J100" s="30">
+        <f t="shared" si="2"/>
+        <v>60.4</v>
+      </c>
+      <c r="M100" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="Y100">
+        <v>73.5</v>
+      </c>
+      <c r="Z100">
+        <v>70.099999999999994</v>
+      </c>
+      <c r="AA100">
         <v>103</v>
       </c>
-      <c r="M97" s="2" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="98" spans="5:13" x14ac:dyDescent="0.25">
-      <c r="E98" s="13">
-        <v>0.11</v>
-      </c>
-      <c r="G98" s="11">
-        <v>51.2</v>
-      </c>
-      <c r="H98" s="20">
+      <c r="AB100">
+        <v>68.900000000000006</v>
+      </c>
+      <c r="AC100">
+        <v>111</v>
+      </c>
+      <c r="AD100">
+        <v>115</v>
+      </c>
+      <c r="AE100">
+        <v>101</v>
+      </c>
+      <c r="AF100">
+        <v>72.3</v>
+      </c>
+      <c r="AG100">
+        <v>48.1</v>
+      </c>
+      <c r="AH100">
+        <v>90</v>
+      </c>
+      <c r="AJ100">
+        <f>AVERAGE(Y100:AH100)</f>
+        <v>85.289999999999992</v>
+      </c>
+      <c r="AK100">
+        <f t="shared" ref="AK100" si="6">G100</f>
+        <v>60.6</v>
+      </c>
+    </row>
+    <row r="101" spans="5:37" x14ac:dyDescent="0.25">
+      <c r="M101" s="2"/>
+    </row>
+    <row r="102" spans="5:37" x14ac:dyDescent="0.25">
+      <c r="M102" s="2" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="103" spans="5:37" x14ac:dyDescent="0.25">
+      <c r="E103" s="12">
+        <v>1.2</v>
+      </c>
+      <c r="G103" s="10">
+        <v>46.2</v>
+      </c>
+      <c r="H103" s="19">
+        <v>0.3</v>
+      </c>
+      <c r="J103" s="30">
+        <f t="shared" si="2"/>
+        <v>45.900000000000006</v>
+      </c>
+      <c r="M103" s="1" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="104" spans="5:37" x14ac:dyDescent="0.25">
+      <c r="E104" s="12">
+        <v>0.24</v>
+      </c>
+      <c r="G104" s="10">
+        <v>57.5</v>
+      </c>
+      <c r="H104" s="19">
+        <v>1.5</v>
+      </c>
+      <c r="J104" s="30">
+        <f t="shared" si="2"/>
+        <v>56</v>
+      </c>
+      <c r="M104" s="1" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="105" spans="5:37" x14ac:dyDescent="0.25">
+      <c r="E105" s="12">
+        <v>0.76</v>
+      </c>
+      <c r="G105" s="10">
+        <v>57.4</v>
+      </c>
+      <c r="H105" s="19">
+        <v>0.4</v>
+      </c>
+      <c r="J105" s="30">
+        <f t="shared" si="2"/>
+        <v>57</v>
+      </c>
+      <c r="M105" s="1" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="106" spans="5:37" x14ac:dyDescent="0.25">
+      <c r="E106" s="12">
         <v>0.8</v>
       </c>
-      <c r="M98" s="1" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="99" spans="5:13" x14ac:dyDescent="0.25">
-      <c r="E99" s="13">
-        <v>0.22</v>
-      </c>
-      <c r="G99" s="11">
-        <v>61.8</v>
-      </c>
-      <c r="H99" s="20">
-        <v>2.8</v>
-      </c>
-      <c r="M99" s="1" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="100" spans="5:13" x14ac:dyDescent="0.25">
-      <c r="E100" s="13">
-        <v>1.2</v>
-      </c>
-      <c r="G100" s="11">
-        <v>60.6</v>
-      </c>
-      <c r="H100" s="20">
-        <v>0.2</v>
-      </c>
-      <c r="M100" s="1" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="101" spans="5:13" x14ac:dyDescent="0.25">
-      <c r="M101" s="2"/>
-    </row>
-    <row r="102" spans="5:13" x14ac:dyDescent="0.25">
-      <c r="M102" s="2" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="103" spans="5:13" x14ac:dyDescent="0.25">
-      <c r="E103" s="13">
-        <v>1.2</v>
-      </c>
-      <c r="G103" s="11">
-        <v>46.34</v>
-      </c>
-      <c r="H103" s="20">
+      <c r="G106" s="10">
+        <v>55.3</v>
+      </c>
+      <c r="H106" s="19">
+        <v>0.3</v>
+      </c>
+      <c r="J106" s="30">
+        <f t="shared" si="2"/>
+        <v>55</v>
+      </c>
+      <c r="M106" s="1" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="107" spans="5:37" x14ac:dyDescent="0.25">
+      <c r="E107" s="12">
+        <v>0.8</v>
+      </c>
+      <c r="G107" s="10">
+        <v>53.6</v>
+      </c>
+      <c r="H107" s="19">
         <v>0</v>
       </c>
-      <c r="M103" s="1" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="104" spans="5:13" x14ac:dyDescent="0.25">
-      <c r="E104" s="13">
-        <v>0.24</v>
-      </c>
-      <c r="G104" s="11">
-        <v>57.5</v>
-      </c>
-      <c r="H104" s="20">
-        <v>1.5</v>
-      </c>
-      <c r="M104" s="1" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="105" spans="5:13" x14ac:dyDescent="0.25">
-      <c r="E105" s="13">
-        <v>0.76</v>
-      </c>
-      <c r="G105" s="11">
-        <v>57.4</v>
-      </c>
-      <c r="H105" s="20">
-        <v>0.4</v>
-      </c>
-      <c r="M105" s="1" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="111" spans="5:13" x14ac:dyDescent="0.25">
+      <c r="J107" s="30">
+        <f t="shared" si="2"/>
+        <v>53.6</v>
+      </c>
+      <c r="M107" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="Y107">
+        <v>59.6</v>
+      </c>
+      <c r="Z107">
+        <v>62.8</v>
+      </c>
+      <c r="AA107">
+        <v>94.1</v>
+      </c>
+      <c r="AB107">
+        <v>59.2</v>
+      </c>
+      <c r="AC107">
+        <v>95.9</v>
+      </c>
+      <c r="AD107">
+        <v>93.2</v>
+      </c>
+      <c r="AE107">
+        <v>83</v>
+      </c>
+      <c r="AF107">
+        <v>45.2</v>
+      </c>
+      <c r="AG107">
+        <v>22.3</v>
+      </c>
+      <c r="AH107">
+        <v>73.7</v>
+      </c>
+      <c r="AJ107">
+        <f>AVERAGE(Y107:AH107)</f>
+        <v>68.900000000000006</v>
+      </c>
+      <c r="AK107">
+        <f t="shared" ref="AK107" si="7">G107</f>
+        <v>53.6</v>
+      </c>
+    </row>
+    <row r="111" spans="5:37" x14ac:dyDescent="0.25">
       <c r="M111" s="2"/>
     </row>
-    <row r="112" spans="5:13" x14ac:dyDescent="0.25">
+    <row r="112" spans="5:37" x14ac:dyDescent="0.25">
       <c r="M112" s="2"/>
     </row>
     <row r="117" spans="4:13" x14ac:dyDescent="0.25">
@@ -2555,14 +2774,14 @@
       <c r="M123" s="2"/>
     </row>
     <row r="124" spans="4:13" x14ac:dyDescent="0.25">
-      <c r="D124" s="14"/>
+      <c r="D124" s="13"/>
       <c r="M124" s="2"/>
     </row>
     <row r="125" spans="4:13" x14ac:dyDescent="0.25">
-      <c r="D125" s="16"/>
+      <c r="D125" s="15"/>
     </row>
     <row r="126" spans="4:13" x14ac:dyDescent="0.25">
-      <c r="D126" s="16"/>
+      <c r="D126" s="15"/>
     </row>
     <row r="128" spans="4:13" x14ac:dyDescent="0.25">
       <c r="M128" s="2"/>
@@ -2571,174 +2790,174 @@
       <c r="M132" s="2"/>
     </row>
     <row r="135" spans="4:13" x14ac:dyDescent="0.25">
-      <c r="F135" s="8"/>
+      <c r="F135" s="7"/>
     </row>
     <row r="140" spans="4:13" x14ac:dyDescent="0.25">
-      <c r="D140" s="17"/>
-      <c r="M140" s="7"/>
+      <c r="D140" s="16"/>
+      <c r="M140" s="6"/>
     </row>
     <row r="141" spans="4:13" x14ac:dyDescent="0.25">
-      <c r="M141" s="7"/>
+      <c r="M141" s="6"/>
     </row>
     <row r="142" spans="4:13" x14ac:dyDescent="0.25">
-      <c r="F142" s="9"/>
-      <c r="M142" s="7"/>
+      <c r="F142" s="8"/>
+      <c r="M142" s="6"/>
     </row>
     <row r="143" spans="4:13" x14ac:dyDescent="0.25">
-      <c r="F143" s="9"/>
-      <c r="M143" s="7"/>
+      <c r="F143" s="8"/>
+      <c r="M143" s="6"/>
     </row>
     <row r="144" spans="4:13" x14ac:dyDescent="0.25">
-      <c r="F144" s="9"/>
-      <c r="M144" s="7"/>
+      <c r="F144" s="8"/>
+      <c r="M144" s="6"/>
     </row>
     <row r="145" spans="6:13" x14ac:dyDescent="0.25">
-      <c r="F145" s="9"/>
-      <c r="M145" s="7"/>
+      <c r="F145" s="8"/>
+      <c r="M145" s="6"/>
     </row>
     <row r="146" spans="6:13" x14ac:dyDescent="0.25">
-      <c r="M146" s="7"/>
+      <c r="M146" s="6"/>
     </row>
     <row r="147" spans="6:13" x14ac:dyDescent="0.25">
-      <c r="F147" s="9"/>
+      <c r="F147" s="8"/>
       <c r="M147" s="2"/>
     </row>
     <row r="148" spans="6:13" x14ac:dyDescent="0.25">
-      <c r="F148" s="9"/>
-      <c r="M148" s="7"/>
+      <c r="F148" s="8"/>
+      <c r="M148" s="6"/>
     </row>
     <row r="149" spans="6:13" x14ac:dyDescent="0.25">
-      <c r="F149" s="9"/>
-      <c r="M149" s="7"/>
+      <c r="F149" s="8"/>
+      <c r="M149" s="6"/>
     </row>
     <row r="150" spans="6:13" x14ac:dyDescent="0.25">
-      <c r="F150" s="9"/>
-      <c r="M150" s="7"/>
+      <c r="F150" s="8"/>
+      <c r="M150" s="6"/>
     </row>
     <row r="151" spans="6:13" x14ac:dyDescent="0.25">
-      <c r="F151" s="9"/>
-      <c r="M151" s="7"/>
+      <c r="F151" s="8"/>
+      <c r="M151" s="6"/>
     </row>
     <row r="152" spans="6:13" x14ac:dyDescent="0.25">
-      <c r="F152" s="9"/>
-      <c r="M152" s="7"/>
+      <c r="F152" s="8"/>
+      <c r="M152" s="6"/>
     </row>
     <row r="153" spans="6:13" x14ac:dyDescent="0.25">
-      <c r="F153" s="9"/>
-      <c r="M153" s="7"/>
+      <c r="F153" s="8"/>
+      <c r="M153" s="6"/>
     </row>
     <row r="154" spans="6:13" x14ac:dyDescent="0.25">
-      <c r="M154" s="7"/>
+      <c r="M154" s="6"/>
     </row>
     <row r="155" spans="6:13" x14ac:dyDescent="0.25">
       <c r="M155" s="2"/>
     </row>
     <row r="156" spans="6:13" x14ac:dyDescent="0.25">
-      <c r="M156" s="7"/>
+      <c r="M156" s="6"/>
     </row>
     <row r="157" spans="6:13" x14ac:dyDescent="0.25">
-      <c r="M157" s="7"/>
+      <c r="M157" s="6"/>
     </row>
     <row r="158" spans="6:13" x14ac:dyDescent="0.25">
-      <c r="M158" s="7"/>
+      <c r="M158" s="6"/>
     </row>
     <row r="159" spans="6:13" x14ac:dyDescent="0.25">
-      <c r="M159" s="7"/>
+      <c r="M159" s="6"/>
     </row>
     <row r="160" spans="6:13" x14ac:dyDescent="0.25">
-      <c r="M160" s="7"/>
+      <c r="M160" s="6"/>
     </row>
     <row r="161" spans="6:13" x14ac:dyDescent="0.25">
       <c r="M161" s="2"/>
     </row>
     <row r="166" spans="6:13" x14ac:dyDescent="0.25">
-      <c r="F166" s="9"/>
+      <c r="F166" s="8"/>
     </row>
     <row r="167" spans="6:13" x14ac:dyDescent="0.25">
-      <c r="F167" s="9"/>
+      <c r="F167" s="8"/>
     </row>
     <row r="168" spans="6:13" x14ac:dyDescent="0.25">
-      <c r="F168" s="9"/>
+      <c r="F168" s="8"/>
     </row>
     <row r="206" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F206" s="9"/>
+      <c r="F206" s="8"/>
     </row>
     <row r="220" spans="13:13" x14ac:dyDescent="0.25">
       <c r="M220" s="2"/>
     </row>
     <row r="226" spans="6:13" x14ac:dyDescent="0.25">
-      <c r="F226" s="9"/>
+      <c r="F226" s="8"/>
     </row>
     <row r="228" spans="6:13" x14ac:dyDescent="0.25">
-      <c r="F228" s="9"/>
+      <c r="F228" s="8"/>
     </row>
     <row r="230" spans="6:13" x14ac:dyDescent="0.25">
-      <c r="F230" s="9"/>
+      <c r="F230" s="8"/>
     </row>
     <row r="232" spans="6:13" x14ac:dyDescent="0.25">
-      <c r="F232" s="9"/>
+      <c r="F232" s="8"/>
     </row>
     <row r="235" spans="6:13" x14ac:dyDescent="0.25">
       <c r="M235" s="2"/>
     </row>
     <row r="271" spans="4:6" x14ac:dyDescent="0.25">
-      <c r="D271" s="18"/>
-      <c r="E271" s="18"/>
-      <c r="F271" s="8"/>
+      <c r="D271" s="17"/>
+      <c r="E271" s="17"/>
+      <c r="F271" s="7"/>
     </row>
     <row r="272" spans="4:6" x14ac:dyDescent="0.25">
-      <c r="D272" s="18"/>
-      <c r="E272" s="18"/>
-      <c r="F272" s="8"/>
+      <c r="D272" s="17"/>
+      <c r="E272" s="17"/>
+      <c r="F272" s="7"/>
     </row>
     <row r="273" spans="4:6" x14ac:dyDescent="0.25">
-      <c r="D273" s="18"/>
-      <c r="E273" s="18"/>
-      <c r="F273" s="8"/>
+      <c r="D273" s="17"/>
+      <c r="E273" s="17"/>
+      <c r="F273" s="7"/>
     </row>
     <row r="274" spans="4:6" x14ac:dyDescent="0.25">
-      <c r="D274" s="18"/>
-      <c r="E274" s="18"/>
-      <c r="F274" s="8"/>
+      <c r="D274" s="17"/>
+      <c r="E274" s="17"/>
+      <c r="F274" s="7"/>
     </row>
     <row r="275" spans="4:6" x14ac:dyDescent="0.25">
-      <c r="D275" s="18"/>
-      <c r="E275" s="18"/>
-      <c r="F275" s="8"/>
+      <c r="D275" s="17"/>
+      <c r="E275" s="17"/>
+      <c r="F275" s="7"/>
     </row>
     <row r="276" spans="4:6" x14ac:dyDescent="0.25">
-      <c r="D276" s="18"/>
-      <c r="E276" s="18"/>
-      <c r="F276" s="8"/>
+      <c r="D276" s="17"/>
+      <c r="E276" s="17"/>
+      <c r="F276" s="7"/>
     </row>
     <row r="277" spans="4:6" x14ac:dyDescent="0.25">
-      <c r="D277" s="18"/>
-      <c r="E277" s="18"/>
-      <c r="F277" s="8"/>
+      <c r="D277" s="17"/>
+      <c r="E277" s="17"/>
+      <c r="F277" s="7"/>
     </row>
     <row r="278" spans="4:6" x14ac:dyDescent="0.25">
-      <c r="D278" s="18"/>
-      <c r="E278" s="18"/>
-      <c r="F278" s="8"/>
+      <c r="D278" s="17"/>
+      <c r="E278" s="17"/>
+      <c r="F278" s="7"/>
     </row>
     <row r="279" spans="4:6" x14ac:dyDescent="0.25">
-      <c r="D279" s="18"/>
-      <c r="E279" s="18"/>
-      <c r="F279" s="8"/>
+      <c r="D279" s="17"/>
+      <c r="E279" s="17"/>
+      <c r="F279" s="7"/>
     </row>
     <row r="280" spans="4:6" x14ac:dyDescent="0.25">
-      <c r="D280" s="18"/>
-      <c r="E280" s="18"/>
-      <c r="F280" s="8"/>
+      <c r="D280" s="17"/>
+      <c r="E280" s="17"/>
+      <c r="F280" s="7"/>
     </row>
     <row r="306" spans="9:9" x14ac:dyDescent="0.25">
-      <c r="I306" s="6"/>
+      <c r="I306" s="5"/>
     </row>
     <row r="307" spans="9:9" x14ac:dyDescent="0.25">
-      <c r="I307" s="6"/>
+      <c r="I307" s="5"/>
     </row>
     <row r="326" spans="9:13" x14ac:dyDescent="0.25">
-      <c r="I326" s="6"/>
+      <c r="I326" s="5"/>
     </row>
     <row r="336" spans="9:13" x14ac:dyDescent="0.25">
       <c r="M336" s="2"/>
@@ -2762,10 +2981,10 @@
       <c r="M392" s="2"/>
     </row>
     <row r="402" spans="13:13" x14ac:dyDescent="0.25">
-      <c r="M402" s="7"/>
+      <c r="M402" s="6"/>
     </row>
     <row r="403" spans="13:13" x14ac:dyDescent="0.25">
-      <c r="M403" s="7"/>
+      <c r="M403" s="6"/>
     </row>
     <row r="404" spans="13:13" x14ac:dyDescent="0.25">
       <c r="M404" s="2"/>
@@ -2774,13 +2993,13 @@
       <c r="M405" s="2"/>
     </row>
     <row r="407" spans="13:13" x14ac:dyDescent="0.25">
-      <c r="M407" s="7"/>
+      <c r="M407" s="6"/>
     </row>
     <row r="408" spans="13:13" x14ac:dyDescent="0.25">
-      <c r="M408" s="7"/>
+      <c r="M408" s="6"/>
     </row>
     <row r="409" spans="13:13" x14ac:dyDescent="0.25">
-      <c r="M409" s="7"/>
+      <c r="M409" s="6"/>
     </row>
     <row r="410" spans="13:13" x14ac:dyDescent="0.25">
       <c r="M410" s="2"/>

</xml_diff>

<commit_message>
Added 24 evaluation cases
</commit_message>
<xml_diff>
--- a/matlab_analysis/Results.xlsx
+++ b/matlab_analysis/Results.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="117">
   <si>
     <t>conf</t>
   </si>
@@ -332,6 +332,39 @@
   </si>
   <si>
     <t>experiment_filenames{82}   = 'Reprint___2014_10_21_noCPD_UCBT_perStep100___2014_10_21_22_15_25';</t>
+  </si>
+  <si>
+    <t>HP_thr</t>
+  </si>
+  <si>
+    <t>HP_samp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">%2014_10_23 henky penky </t>
+  </si>
+  <si>
+    <t>experiment_filenames{83}   = 'Reprint___2014_10_23_changeHP_UCBT_3params_resetSingle___2014_10_23_00_21_19';</t>
+  </si>
+  <si>
+    <t>experiment_filenames{84}   = 'Reprint___2014_10_23_changeHP_UCBT_2params_resetCut___2014_10_23_00_31_18';</t>
+  </si>
+  <si>
+    <t>experiment_filenames{85}   = 'Reprint___2014_10_23_changeHP_UCBT_2params_resetMA___2014_10_23_00_25_45';</t>
+  </si>
+  <si>
+    <t>experiment_filenames{86}   = 'Reprint___2014_10_23_changeHP_UCBT_2params_resetSingle___2014_10_23_00_25_42';</t>
+  </si>
+  <si>
+    <t>experiment_filenames{87}   = 'Reprint___2014_10_23_changeHP_UCBT_2params_resetZero___2014_10_23_00_25_39';</t>
+  </si>
+  <si>
+    <t>vseeno ~ 3000</t>
+  </si>
+  <si>
+    <t>vseeno ~ 2000</t>
+  </si>
+  <si>
+    <t>experiment_filenames{88}   = 'Reprint___2014_10_23_changeHP_UCBT_1par_resetSingleZero___2014_10_23_11_04_28';</t>
   </si>
 </sst>
 </file>
@@ -866,13 +899,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AK422"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="X76" workbookViewId="0">
-      <selection activeCell="AH110" sqref="AH110"/>
+    <sheetView tabSelected="1" topLeftCell="A86" workbookViewId="0">
+      <selection activeCell="N118" sqref="N118"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="5" width="8" style="12" customWidth="1"/>
+    <col min="1" max="2" width="8" style="12" customWidth="1"/>
+    <col min="3" max="3" width="8.85546875" style="12" customWidth="1"/>
+    <col min="4" max="5" width="8" style="12" customWidth="1"/>
     <col min="6" max="6" width="8" customWidth="1"/>
     <col min="7" max="7" width="11.7109375" style="10" customWidth="1"/>
     <col min="8" max="8" width="5.5703125" style="19" customWidth="1"/>
@@ -1990,7 +2025,7 @@
         <v>1.2</v>
       </c>
       <c r="J79" s="30">
-        <f t="shared" ref="J79:J107" si="2">G79-H79</f>
+        <f t="shared" ref="J79:J109" si="2">G79-H79</f>
         <v>61.9</v>
       </c>
       <c r="M79" s="1" t="s">
@@ -2522,7 +2557,7 @@
         <v>56.5</v>
       </c>
     </row>
-    <row r="97" spans="5:37" x14ac:dyDescent="0.25">
+    <row r="97" spans="3:37" x14ac:dyDescent="0.25">
       <c r="E97" s="18" t="s">
         <v>101</v>
       </c>
@@ -2530,7 +2565,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="98" spans="5:37" x14ac:dyDescent="0.25">
+    <row r="98" spans="3:37" x14ac:dyDescent="0.25">
       <c r="E98" s="12">
         <v>0.11</v>
       </c>
@@ -2548,7 +2583,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="99" spans="5:37" x14ac:dyDescent="0.25">
+    <row r="99" spans="3:37" x14ac:dyDescent="0.25">
       <c r="E99" s="12">
         <v>0.22</v>
       </c>
@@ -2566,7 +2601,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="100" spans="5:37" x14ac:dyDescent="0.25">
+    <row r="100" spans="3:37" x14ac:dyDescent="0.25">
       <c r="E100" s="12">
         <v>1.2</v>
       </c>
@@ -2622,15 +2657,60 @@
         <v>60.6</v>
       </c>
     </row>
-    <row r="101" spans="5:37" x14ac:dyDescent="0.25">
+    <row r="101" spans="3:37" x14ac:dyDescent="0.25">
       <c r="M101" s="2"/>
-    </row>
-    <row r="102" spans="5:37" x14ac:dyDescent="0.25">
+      <c r="Y101" s="21" t="s">
+        <v>92</v>
+      </c>
+      <c r="AC101" s="21"/>
+      <c r="AD101" s="21"/>
+      <c r="AE101" s="21"/>
+      <c r="AF101" s="21"/>
+      <c r="AG101" s="21"/>
+      <c r="AH101" s="21"/>
+    </row>
+    <row r="102" spans="3:37" x14ac:dyDescent="0.25">
       <c r="M102" s="2" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="103" spans="5:37" x14ac:dyDescent="0.25">
+      <c r="Y102" s="21">
+        <v>7</v>
+      </c>
+      <c r="Z102" s="21">
+        <v>8</v>
+      </c>
+      <c r="AA102" s="21">
+        <v>9</v>
+      </c>
+      <c r="AB102" s="21">
+        <v>10</v>
+      </c>
+      <c r="AC102" s="21">
+        <v>1</v>
+      </c>
+      <c r="AD102" s="21">
+        <v>2</v>
+      </c>
+      <c r="AE102" s="21">
+        <v>3</v>
+      </c>
+      <c r="AF102" s="21">
+        <v>4</v>
+      </c>
+      <c r="AG102" s="21">
+        <v>5</v>
+      </c>
+      <c r="AH102" s="21">
+        <v>6</v>
+      </c>
+      <c r="AJ102" s="26" t="s">
+        <v>102</v>
+      </c>
+      <c r="AK102" s="23" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="103" spans="3:37" x14ac:dyDescent="0.25">
       <c r="E103" s="12">
         <v>1.2</v>
       </c>
@@ -2648,7 +2728,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="104" spans="5:37" x14ac:dyDescent="0.25">
+    <row r="104" spans="3:37" x14ac:dyDescent="0.25">
       <c r="E104" s="12">
         <v>0.24</v>
       </c>
@@ -2666,7 +2746,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="105" spans="5:37" x14ac:dyDescent="0.25">
+    <row r="105" spans="3:37" x14ac:dyDescent="0.25">
       <c r="E105" s="12">
         <v>0.76</v>
       </c>
@@ -2684,7 +2764,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="106" spans="5:37" x14ac:dyDescent="0.25">
+    <row r="106" spans="3:37" x14ac:dyDescent="0.25">
       <c r="E106" s="12">
         <v>0.8</v>
       </c>
@@ -2702,7 +2782,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="107" spans="5:37" x14ac:dyDescent="0.25">
+    <row r="107" spans="3:37" x14ac:dyDescent="0.25">
       <c r="E107" s="12">
         <v>0.8</v>
       </c>
@@ -2758,32 +2838,254 @@
         <v>53.6</v>
       </c>
     </row>
-    <row r="111" spans="5:37" x14ac:dyDescent="0.25">
-      <c r="M111" s="2"/>
-    </row>
-    <row r="112" spans="5:37" x14ac:dyDescent="0.25">
-      <c r="M112" s="2"/>
-    </row>
-    <row r="117" spans="4:13" x14ac:dyDescent="0.25">
+    <row r="108" spans="3:37" x14ac:dyDescent="0.25">
+      <c r="Y108" s="21" t="s">
+        <v>92</v>
+      </c>
+      <c r="AC108" s="21"/>
+      <c r="AD108" s="21"/>
+      <c r="AE108" s="21"/>
+      <c r="AF108" s="21"/>
+      <c r="AG108" s="21"/>
+      <c r="AH108" s="21"/>
+    </row>
+    <row r="109" spans="3:37" x14ac:dyDescent="0.25">
+      <c r="C109" s="18" t="s">
+        <v>107</v>
+      </c>
+      <c r="D109" s="18" t="s">
+        <v>106</v>
+      </c>
+      <c r="E109" s="18" t="s">
+        <v>101</v>
+      </c>
+      <c r="M109" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="Y109" s="21">
+        <v>7</v>
+      </c>
+      <c r="Z109" s="21">
+        <v>8</v>
+      </c>
+      <c r="AA109" s="21">
+        <v>9</v>
+      </c>
+      <c r="AB109" s="21">
+        <v>10</v>
+      </c>
+      <c r="AC109" s="21">
+        <v>1</v>
+      </c>
+      <c r="AD109" s="21">
+        <v>2</v>
+      </c>
+      <c r="AE109" s="21">
+        <v>3</v>
+      </c>
+      <c r="AF109" s="21">
+        <v>4</v>
+      </c>
+      <c r="AG109" s="21">
+        <v>5</v>
+      </c>
+      <c r="AH109" s="21">
+        <v>6</v>
+      </c>
+      <c r="AJ109" s="26" t="s">
+        <v>102</v>
+      </c>
+      <c r="AK109" s="23" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="110" spans="3:37" x14ac:dyDescent="0.25">
+      <c r="C110" s="17" t="s">
+        <v>115</v>
+      </c>
+      <c r="D110" s="12">
+        <v>40</v>
+      </c>
+      <c r="E110" s="12">
+        <v>0.6</v>
+      </c>
+      <c r="G110" s="10">
+        <v>66.8</v>
+      </c>
+      <c r="H110" s="19">
+        <v>1.6</v>
+      </c>
+      <c r="J110" s="30">
+        <f>G110-H110</f>
+        <v>65.2</v>
+      </c>
+      <c r="M110" s="6" t="s">
+        <v>109</v>
+      </c>
+      <c r="Y110">
+        <v>78.099999999999994</v>
+      </c>
+      <c r="Z110">
+        <v>89.5</v>
+      </c>
+      <c r="AA110">
+        <v>104.1</v>
+      </c>
+      <c r="AB110">
+        <v>76.099999999999994</v>
+      </c>
+      <c r="AC110">
+        <v>115.6</v>
+      </c>
+      <c r="AD110">
+        <v>114.3</v>
+      </c>
+      <c r="AE110">
+        <v>106.9</v>
+      </c>
+      <c r="AF110">
+        <v>76.8</v>
+      </c>
+      <c r="AG110">
+        <v>63</v>
+      </c>
+      <c r="AH110">
+        <v>95.2</v>
+      </c>
+      <c r="AJ110">
+        <f>AVERAGE(Y110:AH110)</f>
+        <v>91.96</v>
+      </c>
+      <c r="AK110">
+        <f t="shared" ref="AK110" si="8">G110</f>
+        <v>66.8</v>
+      </c>
+    </row>
+    <row r="111" spans="3:37" x14ac:dyDescent="0.25">
+      <c r="C111" s="17" t="s">
+        <v>114</v>
+      </c>
+      <c r="D111" s="12">
+        <v>50</v>
+      </c>
+      <c r="G111" s="10">
+        <v>65.099999999999994</v>
+      </c>
+      <c r="H111" s="19">
+        <v>0.9</v>
+      </c>
+      <c r="J111" s="30">
+        <f t="shared" ref="J111:J115" si="9">G111-H111</f>
+        <v>64.199999999999989</v>
+      </c>
+      <c r="M111" s="6" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="112" spans="3:37" x14ac:dyDescent="0.25">
+      <c r="C112" s="17">
+        <v>4000</v>
+      </c>
+      <c r="D112" s="12">
+        <v>43</v>
+      </c>
+      <c r="G112" s="10">
+        <v>64.5</v>
+      </c>
+      <c r="H112" s="19">
+        <v>1</v>
+      </c>
+      <c r="J112" s="30">
+        <f t="shared" si="9"/>
+        <v>63.5</v>
+      </c>
+      <c r="M112" s="6" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="113" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="C113" s="17">
+        <v>3000</v>
+      </c>
+      <c r="D113" s="12">
+        <v>30</v>
+      </c>
+      <c r="G113" s="10">
+        <v>64.400000000000006</v>
+      </c>
+      <c r="H113" s="19">
+        <v>0.5</v>
+      </c>
+      <c r="J113" s="30">
+        <f t="shared" si="9"/>
+        <v>63.900000000000006</v>
+      </c>
+      <c r="M113" s="6" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="114" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="C114" s="17"/>
+      <c r="D114" s="12">
+        <v>45</v>
+      </c>
+      <c r="G114" s="10">
+        <v>63.3</v>
+      </c>
+      <c r="H114" s="19">
+        <v>0.2</v>
+      </c>
+      <c r="J114" s="30">
+        <f t="shared" si="9"/>
+        <v>63.099999999999994</v>
+      </c>
+      <c r="M114" s="1" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="115" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="C115" s="17"/>
+      <c r="D115" s="12">
+        <v>40</v>
+      </c>
+      <c r="G115" s="10">
+        <v>65.5</v>
+      </c>
+      <c r="H115" s="19">
+        <v>0.5</v>
+      </c>
+      <c r="J115" s="30">
+        <f t="shared" si="9"/>
+        <v>65</v>
+      </c>
+      <c r="M115" s="1" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="116" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="C116" s="17"/>
+    </row>
+    <row r="117" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="C117" s="17"/>
       <c r="M117" s="2"/>
     </row>
-    <row r="118" spans="4:13" x14ac:dyDescent="0.25">
+    <row r="118" spans="3:13" x14ac:dyDescent="0.25">
       <c r="M118" s="2"/>
     </row>
-    <row r="123" spans="4:13" x14ac:dyDescent="0.25">
+    <row r="123" spans="3:13" x14ac:dyDescent="0.25">
       <c r="M123" s="2"/>
     </row>
-    <row r="124" spans="4:13" x14ac:dyDescent="0.25">
+    <row r="124" spans="3:13" x14ac:dyDescent="0.25">
       <c r="D124" s="13"/>
       <c r="M124" s="2"/>
     </row>
-    <row r="125" spans="4:13" x14ac:dyDescent="0.25">
+    <row r="125" spans="3:13" x14ac:dyDescent="0.25">
       <c r="D125" s="15"/>
     </row>
-    <row r="126" spans="4:13" x14ac:dyDescent="0.25">
+    <row r="126" spans="3:13" x14ac:dyDescent="0.25">
       <c r="D126" s="15"/>
     </row>
-    <row r="128" spans="4:13" x14ac:dyDescent="0.25">
+    <row r="128" spans="3:13" x14ac:dyDescent="0.25">
       <c r="M128" s="2"/>
     </row>
     <row r="132" spans="4:13" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Added experiments for fixed parameters evaluation Added first results from fixed parameters evaluation
</commit_message>
<xml_diff>
--- a/matlab_analysis/Results.xlsx
+++ b/matlab_analysis/Results.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="118">
   <si>
     <t>conf</t>
   </si>
@@ -365,6 +365,9 @@
   </si>
   <si>
     <t>experiment_filenames{88}   = 'Reprint___2014_10_23_changeHP_UCBT_1par_resetSingleZero___2014_10_23_11_04_28';</t>
+  </si>
+  <si>
+    <t>mislim da je to narobe bil indeks v meritvah (parameter je bil dejansko fiksiran na 50)</t>
   </si>
 </sst>
 </file>
@@ -533,7 +536,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -591,6 +594,9 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="164" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
   </cellXfs>
@@ -899,8 +905,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AK422"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A86" workbookViewId="0">
-      <selection activeCell="N118" sqref="N118"/>
+    <sheetView tabSelected="1" topLeftCell="A96" workbookViewId="0">
+      <selection activeCell="C109" sqref="C109"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2025,7 +2031,7 @@
         <v>1.2</v>
       </c>
       <c r="J79" s="30">
-        <f t="shared" ref="J79:J109" si="2">G79-H79</f>
+        <f t="shared" ref="J79:J107" si="2">G79-H79</f>
         <v>61.9</v>
       </c>
       <c r="M79" s="1" t="s">
@@ -2839,6 +2845,9 @@
       </c>
     </row>
     <row r="108" spans="3:37" x14ac:dyDescent="0.25">
+      <c r="C108" s="15" t="s">
+        <v>117</v>
+      </c>
       <c r="Y108" s="21" t="s">
         <v>92</v>
       </c>
@@ -2850,7 +2859,7 @@
       <c r="AH108" s="21"/>
     </row>
     <row r="109" spans="3:37" x14ac:dyDescent="0.25">
-      <c r="C109" s="18" t="s">
+      <c r="C109" s="15" t="s">
         <v>107</v>
       </c>
       <c r="D109" s="18" t="s">
@@ -2900,7 +2909,7 @@
       </c>
     </row>
     <row r="110" spans="3:37" x14ac:dyDescent="0.25">
-      <c r="C110" s="17" t="s">
+      <c r="C110" s="31" t="s">
         <v>115</v>
       </c>
       <c r="D110" s="12">
@@ -2962,7 +2971,7 @@
       </c>
     </row>
     <row r="111" spans="3:37" x14ac:dyDescent="0.25">
-      <c r="C111" s="17" t="s">
+      <c r="C111" s="31" t="s">
         <v>114</v>
       </c>
       <c r="D111" s="12">
@@ -2983,7 +2992,7 @@
       </c>
     </row>
     <row r="112" spans="3:37" x14ac:dyDescent="0.25">
-      <c r="C112" s="17">
+      <c r="C112" s="31">
         <v>4000</v>
       </c>
       <c r="D112" s="12">
@@ -3004,7 +3013,7 @@
       </c>
     </row>
     <row r="113" spans="3:13" x14ac:dyDescent="0.25">
-      <c r="C113" s="17">
+      <c r="C113" s="31">
         <v>3000</v>
       </c>
       <c r="D113" s="12">

</xml_diff>